<commit_message>
Consultas en SQL para principiantes
</commit_message>
<xml_diff>
--- a/00soportes/Ruta Desarrollo Web.xlsx
+++ b/00soportes/Ruta Desarrollo Web.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\cvpetrix2022\00soportes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8F551D-9BEE-4691-A9D9-2ED41ECA5660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6250C3BE-B689-4034-8D59-579F23E31915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4251" uniqueCount="1347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4269" uniqueCount="1354">
   <si>
     <t>id</t>
   </si>
@@ -4088,6 +4088,27 @@
   </si>
   <si>
     <t>Aprende Laravel 10 desde cero y conviértete en un experto en el framework PHP más popular. Construye aplicaciones web escalables y descubre las mejores prácticas y técnicas de Laravel. ¡Inscríbete ahora!</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/sql-desde-cero-curso-practico</t>
+  </si>
+  <si>
+    <t>Consultas en SQL para principiantes</t>
+  </si>
+  <si>
+    <t>https://github.com/petrix12/repasosql.git</t>
+  </si>
+  <si>
+    <t>UC-72f027a7-64ce-4f9e-b371-5a2ef0102b0d</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/certificate/UC-72f027a7-64ce-4f9e-b371-5a2ef0102b0d</t>
+  </si>
+  <si>
+    <t>Jorge, con experiencia en bases de datos, te enseñará SQL desde cero.</t>
+  </si>
+  <si>
+    <t>Jorge Alberto Chávez Sarmiento</t>
   </si>
 </sst>
 </file>
@@ -4242,6 +4263,27 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -4258,13 +4300,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
@@ -4299,20 +4334,6 @@
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
       </font>
     </dxf>
   </dxfs>
@@ -5901,24 +5922,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{35821B52-E1A3-4F68-8264-95586991A61F}" name="Tabla5" displayName="Tabla5" ref="A1:Y248" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:Y248" xr:uid="{35821B52-E1A3-4F68-8264-95586991A61F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{35821B52-E1A3-4F68-8264-95586991A61F}" name="Tabla5" displayName="Tabla5" ref="A1:Y249" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A1:Y249" xr:uid="{35821B52-E1A3-4F68-8264-95586991A61F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:X167">
     <sortCondition ref="A1:A167"/>
   </sortState>
   <tableColumns count="25">
-    <tableColumn id="1" xr3:uid="{6EC704AD-AD44-4DB4-918A-B83D695DE3A1}" name="id" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{6EC704AD-AD44-4DB4-918A-B83D695DE3A1}" name="id" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{B6F432CE-A60E-4F0D-A068-BDBB9D7A889D}" name="name"/>
     <tableColumn id="3" xr3:uid="{CBF16A43-3D5D-48FC-889C-DDFFC90864C6}" name="category"/>
     <tableColumn id="4" xr3:uid="{A413336C-15DF-455C-AE67-3338C4704783}" name="technology"/>
     <tableColumn id="5" xr3:uid="{60D649E9-0DAB-4D18-A438-7540D6003181}" name="url"/>
     <tableColumn id="6" xr3:uid="{9830F84C-0142-4D75-BB99-D04B24D36BF1}" name="platform"/>
-    <tableColumn id="7" xr3:uid="{E2ACB74C-7FD5-4AD9-83E2-4A21192DB0D4}" name="costo" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{E2ACB74C-7FD5-4AD9-83E2-4A21192DB0D4}" name="costo" dataDxfId="7"/>
     <tableColumn id="8" xr3:uid="{44ECA173-471E-42B1-AA33-2E4923E72500}" name="money"/>
     <tableColumn id="9" xr3:uid="{47CD3EE7-ACA8-4A3C-954B-5ED7DDEE8E2E}" name="comprado"/>
-    <tableColumn id="10" xr3:uid="{67D3F461-8DCC-49E8-A6CC-61700C7F7434}" name="priority" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{67D3F461-8DCC-49E8-A6CC-61700C7F7434}" name="priority" dataDxfId="6"/>
     <tableColumn id="11" xr3:uid="{1BF73A1E-992B-4FA8-A326-8402B55BBD45}" name="minutos"/>
-    <tableColumn id="12" xr3:uid="{C44892B3-5714-4E96-B162-9A8BF12FA266}" name="culminado" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{C44892B3-5714-4E96-B162-9A8BF12FA266}" name="culminado" dataDxfId="5"/>
     <tableColumn id="13" xr3:uid="{B33C3B66-DCC5-474F-8411-717696A1EEB4}" name="certificado"/>
     <tableColumn id="14" xr3:uid="{B307D051-5313-444F-B8D4-2A761D46142F}" name="url_certificado"/>
     <tableColumn id="15" xr3:uid="{70045D3A-385B-4A70-9539-C1590FCD0123}" name="instructor"/>
@@ -5938,10 +5959,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{067E9773-6429-4990-A4BC-176AC8A0C3C6}" name="Tabla4" displayName="Tabla4" ref="A1:B143" totalsRowShown="0">
-  <autoFilter ref="A1:B143" xr:uid="{067E9773-6429-4990-A4BC-176AC8A0C3C6}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B142">
-    <sortCondition ref="B1:B142"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{067E9773-6429-4990-A4BC-176AC8A0C3C6}" name="Tabla4" displayName="Tabla4" ref="A1:B144" totalsRowShown="0">
+  <autoFilter ref="A1:B144" xr:uid="{067E9773-6429-4990-A4BC-176AC8A0C3C6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B144">
+    <sortCondition ref="B1:B144"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A8E3C3EB-511E-4761-B90D-E66FDBAF1766}" name="id"/>
@@ -5952,7 +5973,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F538BEF-BAAF-40F0-934B-EC148983A715}" name="Tabla1" displayName="Tabla1" ref="A1:B22" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F538BEF-BAAF-40F0-934B-EC148983A715}" name="Tabla1" displayName="Tabla1" ref="A1:B22" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:B22" xr:uid="{6F538BEF-BAAF-40F0-934B-EC148983A715}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B22">
     <sortCondition ref="B1:B22"/>
@@ -6261,8 +6282,8 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6276,7 +6297,7 @@
       </c>
       <c r="B1" s="13">
         <f ca="1">TODAY()</f>
-        <v>45131</v>
+        <v>45195</v>
       </c>
       <c r="E1" s="21">
         <f>SUMIF(courses!J:J,1,courses!K:K)/60</f>
@@ -6362,7 +6383,7 @@
       </c>
       <c r="F5" s="15">
         <f ca="1">SUMIFS(courses!$K:$K,courses!$C:$C,Dashboard!$A5,courses!$L:$L,"&gt;=1-1-"&amp;F$3,courses!$L:$L,"&lt;=31-12-"&amp;F$3)/60</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -6862,7 +6883,7 @@
       </c>
       <c r="F25" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>33.566666666666663</v>
+        <v>39.06666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -6876,13 +6897,13 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:AZ248"/>
+  <dimension ref="A1:AZ249"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="Q239" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AZ248" sqref="AZ2:AZ248"/>
+      <selection pane="bottomRight" activeCell="V252" sqref="V252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48458,16 +48479,189 @@
         <v>nota: ''</v>
       </c>
       <c r="AZ248" t="str">
-        <f t="shared" ref="AZ248" si="32">"{ "&amp;AA248&amp;AB248&amp;AC248&amp;AD248&amp;AE248&amp;AF248&amp;AG248&amp;AH248&amp;AI248&amp;AJ248&amp;AK248&amp;AL248&amp;AM248&amp;AN248&amp;AO248&amp;AP248&amp;AQ248&amp;AR248&amp;AS248&amp;AT248&amp;AU248&amp;AV248&amp;AW248&amp;AX248&amp;AY248&amp;" },"</f>
+        <f t="shared" ref="AZ248:AZ249" si="32">"{ "&amp;AA248&amp;AB248&amp;AC248&amp;AD248&amp;AE248&amp;AF248&amp;AG248&amp;AH248&amp;AI248&amp;AJ248&amp;AK248&amp;AL248&amp;AM248&amp;AN248&amp;AO248&amp;AP248&amp;AQ248&amp;AR248&amp;AS248&amp;AT248&amp;AU248&amp;AV248&amp;AW248&amp;AX248&amp;AY248&amp;" },"</f>
         <v>{ id: 247, name: 'Aprende Laravel 10 desde cero', category: 'Frameworks de back-end', technology: 'Laravel', url: 'https://codersfree.com/cursos/aprende-laravel-desde-cero', platform: 'Coders Free', costo: 0, money: 'USD', comprado: false, priority: 0, minutos: 1332, culminado: '2023-07-24', certificado: 'S/C', url_certificado: '', instructor: 'Victor Arana Flores', description: 'Aprende Laravel 10 desde cero y conviértete en un experto en el framework PHP más popular. Construye aplicaciones web escalables y descubre las mejores prácticas y técnicas de Laravel. ¡Inscríbete ahora!', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: false, logo_platform: 'coders_free', logo_technologies: [ 'laravel' ], mostrar: true, repositorio: '', nota: '' },</v>
+      </c>
+    </row>
+    <row r="249" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A249" s="6">
+        <v>248</v>
+      </c>
+      <c r="B249" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C249" t="s">
+        <v>374</v>
+      </c>
+      <c r="D249" t="s">
+        <v>509</v>
+      </c>
+      <c r="E249" s="2" t="s">
+        <v>1347</v>
+      </c>
+      <c r="F249" t="s">
+        <v>8</v>
+      </c>
+      <c r="G249" s="3">
+        <v>0</v>
+      </c>
+      <c r="H249" t="s">
+        <v>47</v>
+      </c>
+      <c r="I249" t="s">
+        <v>15</v>
+      </c>
+      <c r="J249" s="4">
+        <v>0</v>
+      </c>
+      <c r="K249">
+        <f>5.5*60</f>
+        <v>330</v>
+      </c>
+      <c r="L249" s="9">
+        <v>45195</v>
+      </c>
+      <c r="M249" t="s">
+        <v>1350</v>
+      </c>
+      <c r="N249" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="O249" t="s">
+        <v>1353</v>
+      </c>
+      <c r="P249" t="s">
+        <v>1352</v>
+      </c>
+      <c r="S249" t="s">
+        <v>14</v>
+      </c>
+      <c r="T249" t="s">
+        <v>14</v>
+      </c>
+      <c r="U249" t="s">
+        <v>783</v>
+      </c>
+      <c r="V249" s="19" t="s">
+        <v>858</v>
+      </c>
+      <c r="W249" t="s">
+        <v>14</v>
+      </c>
+      <c r="X249" s="2" t="s">
+        <v>1349</v>
+      </c>
+      <c r="AA249" t="str">
+        <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
+        <v xml:space="preserve">id: 248, </v>
+      </c>
+      <c r="AB249" t="str">
+        <f>AB$1&amp;": '"&amp;Tabla5[[#This Row],[name]]&amp;"', "</f>
+        <v xml:space="preserve">name: 'Consultas en SQL para principiantes', </v>
+      </c>
+      <c r="AC249" t="str">
+        <f>AC$1&amp;": '"&amp;Tabla5[[#This Row],[category]]&amp;"', "</f>
+        <v xml:space="preserve">category: 'Bases de datos', </v>
+      </c>
+      <c r="AD249" t="str">
+        <f>AD$1&amp;": '"&amp;Tabla5[[#This Row],[technology]]&amp;"', "</f>
+        <v xml:space="preserve">technology: 'SQL', </v>
+      </c>
+      <c r="AE249" t="str">
+        <f>AE$1&amp;": '"&amp;Tabla5[[#This Row],[url]]&amp;"', "</f>
+        <v xml:space="preserve">url: 'https://www.udemy.com/course/sql-desde-cero-curso-practico', </v>
+      </c>
+      <c r="AF249" t="str">
+        <f>AF$1&amp;": '"&amp;Tabla5[[#This Row],[platform]]&amp;"', "</f>
+        <v xml:space="preserve">platform: 'Udemy', </v>
+      </c>
+      <c r="AG249" t="str">
+        <f>AG$1&amp;": "&amp;SUBSTITUTE(Tabla5[[#This Row],[costo]],",",".")&amp;", "</f>
+        <v xml:space="preserve">costo: 0, </v>
+      </c>
+      <c r="AH249" t="str">
+        <f>AH$1&amp;": '"&amp;Tabla5[[#This Row],[money]]&amp;"', "</f>
+        <v xml:space="preserve">money: 'USD', </v>
+      </c>
+      <c r="AI249" t="str">
+        <f>AI$1&amp;": "&amp;Tabla5[[#This Row],[comprado]]&amp;", "</f>
+        <v xml:space="preserve">comprado: false, </v>
+      </c>
+      <c r="AJ249" t="str">
+        <f>AJ$1&amp;": "&amp;Tabla5[[#This Row],[priority]]&amp;", "</f>
+        <v xml:space="preserve">priority: 0, </v>
+      </c>
+      <c r="AK249" t="str">
+        <f>AK$1&amp;": "&amp;Tabla5[[#This Row],[minutos]]&amp;", "</f>
+        <v xml:space="preserve">minutos: 330, </v>
+      </c>
+      <c r="AL249" t="str">
+        <f>AL$1&amp;": "&amp;IF(Tabla5[[#This Row],[culminado]]=0,"null","'"&amp;TEXT(Tabla5[[#This Row],[culminado]],"aaaa-mm-dd")&amp;"'")&amp;", "</f>
+        <v xml:space="preserve">culminado: '2023-09-26', </v>
+      </c>
+      <c r="AM249" t="str">
+        <f>AM$1&amp;": '"&amp;Tabla5[[#This Row],[certificado]]&amp;"', "</f>
+        <v xml:space="preserve">certificado: 'UC-72f027a7-64ce-4f9e-b371-5a2ef0102b0d', </v>
+      </c>
+      <c r="AN249" t="str">
+        <f>AN$1&amp;": '"&amp;Tabla5[[#This Row],[url_certificado]]&amp;"', "</f>
+        <v xml:space="preserve">url_certificado: 'https://www.udemy.com/certificate/UC-72f027a7-64ce-4f9e-b371-5a2ef0102b0d', </v>
+      </c>
+      <c r="AO249" t="str">
+        <f>AO$1&amp;": '"&amp;Tabla5[[#This Row],[instructor]]&amp;"', "</f>
+        <v xml:space="preserve">instructor: 'Jorge Alberto Chávez Sarmiento', </v>
+      </c>
+      <c r="AP249" t="str">
+        <f>AP$1&amp;": '"&amp;Tabla5[[#This Row],[description]]&amp;"', "</f>
+        <v xml:space="preserve">description: 'Jorge, con experiencia en bases de datos, te enseñará SQL desde cero.', </v>
+      </c>
+      <c r="AQ249" t="str">
+        <f>AQ$1&amp;": '"&amp;Tabla5[[#This Row],[url_aux]]&amp;"', "</f>
+        <v xml:space="preserve">url_aux: '', </v>
+      </c>
+      <c r="AR249" t="str">
+        <f>AR$1&amp;": '"&amp;Tabla5[[#This Row],[calificacion]]&amp;"', "</f>
+        <v xml:space="preserve">calificacion: '', </v>
+      </c>
+      <c r="AS249" t="str">
+        <f>AS$1&amp;": "&amp;Tabla5[[#This Row],[actualizado]]&amp;", "</f>
+        <v xml:space="preserve">actualizado: true, </v>
+      </c>
+      <c r="AT249" t="str">
+        <f>AT$1&amp;": "&amp;Tabla5[[#This Row],[en_ruta]]&amp;", "</f>
+        <v xml:space="preserve">en_ruta: true, </v>
+      </c>
+      <c r="AU249" t="str">
+        <f>AU$1&amp;": '"&amp;Tabla5[[#This Row],[logo_platform]]&amp;"', "</f>
+        <v xml:space="preserve">logo_platform: 'udemy', </v>
+      </c>
+      <c r="AV249" t="str">
+        <f>AV$1&amp;": [ "&amp;Tabla5[[#This Row],[logo_technologies]]&amp;" ], "</f>
+        <v xml:space="preserve">logo_technologies: [ 'sql' ], </v>
+      </c>
+      <c r="AW249" t="str">
+        <f>AW$1&amp;": "&amp;Tabla5[[#This Row],[mostrar]]&amp;", "</f>
+        <v xml:space="preserve">mostrar: true, </v>
+      </c>
+      <c r="AX249" t="str">
+        <f>AX$1&amp;": '"&amp;Tabla5[[#This Row],[repositorio]]&amp;"', "</f>
+        <v xml:space="preserve">repositorio: 'https://github.com/petrix12/repasosql.git', </v>
+      </c>
+      <c r="AY249" t="str">
+        <f>AY$1&amp;": '"&amp;Tabla5[[#This Row],[nota]]&amp;"'"</f>
+        <v>nota: ''</v>
+      </c>
+      <c r="AZ249" t="str">
+        <f t="shared" ref="AZ249" si="33">"{ "&amp;AA249&amp;AB249&amp;AC249&amp;AD249&amp;AE249&amp;AF249&amp;AG249&amp;AH249&amp;AI249&amp;AJ249&amp;AK249&amp;AL249&amp;AM249&amp;AN249&amp;AO249&amp;AP249&amp;AQ249&amp;AR249&amp;AS249&amp;AT249&amp;AU249&amp;AV249&amp;AW249&amp;AX249&amp;AY249&amp;" },"</f>
+        <v>{ id: 248, name: 'Consultas en SQL para principiantes', category: 'Bases de datos', technology: 'SQL', url: 'https://www.udemy.com/course/sql-desde-cero-curso-practico', platform: 'Udemy', costo: 0, money: 'USD', comprado: false, priority: 0, minutos: 330, culminado: '2023-09-26', certificado: 'UC-72f027a7-64ce-4f9e-b371-5a2ef0102b0d', url_certificado: 'https://www.udemy.com/certificate/UC-72f027a7-64ce-4f9e-b371-5a2ef0102b0d', instructor: 'Jorge Alberto Chávez Sarmiento', description: 'Jorge, con experiencia en bases de datos, te enseñará SQL desde cero.', url_aux: '', calificacion: '', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'sql' ], mostrar: true, repositorio: 'https://github.com/petrix12/repasosql.git', nota: '' },</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{EFDDBBC5-452A-4BC6-A598-4F0D98E92E23}">
@@ -48476,7 +48670,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{080BBF38-91CF-44A2-8034-B83AEB3677D2}">
       <formula1>platform</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576 S2:T1048576 W2:W1048576" xr:uid="{678243B2-4193-4FA8-A190-37A986A340CF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W1048576 I2:I1048576 S2:T1048576" xr:uid="{678243B2-4193-4FA8-A190-37A986A340CF}">
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{FA3C4A9B-80C8-4335-B4E6-A3C8412DC1E8}">
@@ -48818,11 +49012,14 @@
     <hyperlink ref="E247" r:id="rId323" xr:uid="{2BC4B64E-3262-4788-9F8F-9FF8035C15FB}"/>
     <hyperlink ref="X247" r:id="rId324" xr:uid="{13129819-2040-42DC-8DEF-ADA241E259E6}"/>
     <hyperlink ref="E248" r:id="rId325" xr:uid="{3DC12900-1075-4076-B710-6B02064C9AC4}"/>
+    <hyperlink ref="E249" r:id="rId326" xr:uid="{35162861-0AB7-461D-B4E4-99A52CAA8FC7}"/>
+    <hyperlink ref="X249" r:id="rId327" xr:uid="{1E50BA9E-45B5-4649-802D-947D937A4C91}"/>
+    <hyperlink ref="N249" r:id="rId328" xr:uid="{6D0A4449-DC34-4A8D-885F-4EC745E919BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId326"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId329"/>
   <tableParts count="1">
-    <tablePart r:id="rId327"/>
+    <tablePart r:id="rId330"/>
   </tableParts>
 </worksheet>
 </file>
@@ -48865,13 +49062,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621B7A30-42A9-465B-AA2D-305E3F2C1EE1}">
-  <dimension ref="A1:B143"/>
+  <dimension ref="A1:B144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B129" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A144" sqref="A144"/>
+      <selection pane="bottomRight" activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49449,583 +49646,591 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B72" t="s">
-        <v>1164</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B73" t="s">
-        <v>76</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="B74" t="s">
-        <v>730</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="B75" t="s">
-        <v>87</v>
+        <v>730</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B76" t="s">
-        <v>583</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B77" t="s">
-        <v>148</v>
+        <v>583</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>124</v>
+        <v>58</v>
       </c>
       <c r="B78" t="s">
-        <v>1057</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="B79" t="s">
-        <v>155</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B80" t="s">
-        <v>566</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B81" t="s">
-        <v>346</v>
+        <v>566</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B82" t="s">
-        <v>431</v>
+        <v>346</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>131</v>
+        <v>62</v>
       </c>
       <c r="B83" t="s">
-        <v>1189</v>
+        <v>431</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B84" t="s">
-        <v>1157</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="B85" t="s">
-        <v>160</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B86" t="s">
-        <v>105</v>
+        <v>160</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>135</v>
+        <v>64</v>
       </c>
       <c r="B87" t="s">
-        <v>1228</v>
+        <v>105</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="B88" t="s">
-        <v>719</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="B89" t="s">
-        <v>550</v>
+        <v>719</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B90" t="s">
-        <v>31</v>
+        <v>550</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B91" t="s">
-        <v>229</v>
+        <v>31</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B92" t="s">
-        <v>159</v>
+        <v>229</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B93" t="s">
-        <v>244</v>
+        <v>159</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B94" t="s">
-        <v>403</v>
+        <v>244</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="B95" t="s">
-        <v>709</v>
+        <v>403</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B96" t="s">
-        <v>752</v>
+        <v>709</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="B97" t="s">
-        <v>36</v>
+        <v>752</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B98" t="s">
-        <v>111</v>
+        <v>36</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
+        <v>72</v>
+      </c>
+      <c r="B99" t="s">
         <v>111</v>
-      </c>
-      <c r="B99" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="B100" t="s">
-        <v>365</v>
+        <v>733</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B101" t="s">
-        <v>623</v>
+        <v>365</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B102" t="s">
-        <v>138</v>
+        <v>623</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B103" t="s">
-        <v>70</v>
+        <v>138</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>77</v>
+        <v>142</v>
       </c>
       <c r="B104" t="s">
-        <v>33</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B105" t="s">
-        <v>505</v>
+        <v>70</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>139</v>
+        <v>77</v>
       </c>
       <c r="B106" t="s">
-        <v>1265</v>
+        <v>33</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B107" t="s">
-        <v>86</v>
+        <v>505</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="B108" t="s">
-        <v>299</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>141</v>
+        <v>79</v>
       </c>
       <c r="B109" t="s">
-        <v>1278</v>
+        <v>86</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>127</v>
+        <v>80</v>
       </c>
       <c r="B110" t="s">
-        <v>1161</v>
+        <v>299</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>113</v>
+        <v>141</v>
       </c>
       <c r="B111" t="s">
-        <v>736</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B112" t="s">
-        <v>819</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>103</v>
+        <v>736</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="B114" t="s">
-        <v>464</v>
+        <v>819</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B115" t="s">
-        <v>355</v>
+        <v>103</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>130</v>
+        <v>82</v>
       </c>
       <c r="B116" t="s">
-        <v>1176</v>
+        <v>464</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B117" t="s">
-        <v>562</v>
+        <v>355</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="B118" t="s">
-        <v>727</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B119" t="s">
-        <v>85</v>
+        <v>562</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B120" t="s">
-        <v>1148</v>
+        <v>727</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B121" t="s">
-        <v>130</v>
+        <v>85</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="B122" t="s">
-        <v>725</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="B123" t="s">
-        <v>755</v>
+        <v>130</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="B124" t="s">
-        <v>477</v>
+        <v>725</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="B125" t="s">
-        <v>174</v>
+        <v>755</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B126" t="s">
-        <v>666</v>
+        <v>477</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B127" t="s">
-        <v>645</v>
+        <v>174</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B128" t="s">
-        <v>307</v>
+        <v>666</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B129" t="s">
-        <v>185</v>
+        <v>645</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="B130" t="s">
-        <v>821</v>
+        <v>307</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B131" t="s">
-        <v>1058</v>
+        <v>185</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="B132" t="s">
-        <v>108</v>
+        <v>821</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B133" t="s">
-        <v>150</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B134" t="s">
-        <v>209</v>
+        <v>108</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="B135" t="s">
-        <v>1170</v>
+        <v>150</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="B136" t="s">
-        <v>1171</v>
+        <v>209</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="B137" t="s">
-        <v>117</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="B138" t="s">
-        <v>603</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B139" t="s">
-        <v>265</v>
+        <v>117</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B140" t="s">
-        <v>82</v>
+        <v>603</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="B141" t="s">
-        <v>1209</v>
+        <v>265</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>138</v>
+        <v>99</v>
       </c>
       <c r="B142" t="s">
-        <v>1260</v>
+        <v>82</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B143" t="s">
-        <v>1326</v>
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>138</v>
+      </c>
+      <c r="B144" t="s">
+        <v>1260</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
curso avanzado de laravel 11
</commit_message>
<xml_diff>
--- a/00soportes/Ruta Desarrollo Web.xlsx
+++ b/00soportes/Ruta Desarrollo Web.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\cvpetrix2022\00soportes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D20247-90D2-4BF5-859E-E359A6B4AF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECDE4E6-EF37-4381-B394-A31FA89CA938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4319" uniqueCount="1367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4351" uniqueCount="1373">
   <si>
     <t>id</t>
   </si>
@@ -4147,7 +4147,25 @@
     <t>Juan José Ruíz Muñoz</t>
   </si>
   <si>
-    <t>arquitectura_hexagonal'</t>
+    <t>Novedades de Laravel 10</t>
+  </si>
+  <si>
+    <t>https://aprendible.com/series/novedades-de-laravel-10</t>
+  </si>
+  <si>
+    <t>En esta serie de videos exploramos las principales novedades de la versión 10 de Laravel liberada el 14 de febrero del 2023.</t>
+  </si>
+  <si>
+    <t>Curso avanzado de Laravel 11</t>
+  </si>
+  <si>
+    <t>https://codersfree.com/cursos/aprende-laravel-avanzado</t>
+  </si>
+  <si>
+    <t>En este curso avanzado de Laravel 11, aprenderás técnicas y herramientas avanzadas para mejorar tus habilidades en Laravel. Domina Laravel y crea aplicaciones web de alta calidad.</t>
+  </si>
+  <si>
+    <t>'arquitectura_hexagonal'</t>
   </si>
 </sst>
 </file>
@@ -5961,14 +5979,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{35821B52-E1A3-4F68-8264-95586991A61F}" name="Tabla5" displayName="Tabla5" ref="A1:Y252" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:Y252" xr:uid="{35821B52-E1A3-4F68-8264-95586991A61F}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Laravel"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{35821B52-E1A3-4F68-8264-95586991A61F}" name="Tabla5" displayName="Tabla5" ref="A1:Y254" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A1:Y254" xr:uid="{35821B52-E1A3-4F68-8264-95586991A61F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:X167">
     <sortCondition ref="A1:A167"/>
   </sortState>
@@ -6342,7 +6354,7 @@
       </c>
       <c r="B1" s="13">
         <f ca="1">TODAY()</f>
-        <v>45374</v>
+        <v>45457</v>
       </c>
       <c r="E1" s="21">
         <f>SUMIF(courses!J:J,1,courses!K:K)/60</f>
@@ -6553,7 +6565,7 @@
       </c>
       <c r="F10" s="15">
         <f ca="1">SUMIFS(courses!$K:$K,courses!$C:$C,Dashboard!$A10,courses!$L:$L,"&gt;=1-1-"&amp;F$3,courses!$L:$L,"&lt;=31-12-"&amp;F$3)/60</f>
-        <v>4.3166666666666664</v>
+        <v>39.75</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -6928,7 +6940,7 @@
       </c>
       <c r="F25" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>5.1666666666666661</v>
+        <v>40.6</v>
       </c>
     </row>
   </sheetData>
@@ -6942,13 +6954,13 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:AZ252"/>
+  <dimension ref="A1:AZ254"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="Q141" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="R245" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA254" sqref="AA254"/>
+      <selection pane="bottomRight" activeCell="V253" sqref="V253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7131,7 +7143,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="2" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -7295,7 +7307,7 @@
         <v>{ id: 1, name: 'Visual Studio Code: Mejora tu velocidad para codificar', category: 'Herramientas', technology: 'VS Code', url: 'https://www.udemy.com/course/vscode-mejora-tu-velocidad-para-codificar', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 104, culminado: null, certificado: '', url_certificado: '', instructor: 'Fernando Herrera', description: 'Trucos que te harán disfrutar más tu experiencia como desarrollador y trabajar a mayor velocidad en VSCode.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'vsc' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="3" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -7459,7 +7471,7 @@
         <v>{ id: 2, name: 'Git desde cero!', category: 'Herramientas', technology: 'Git', url: 'https://www.udemy.com/course/git-desde-cero', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 102, culminado: null, certificado: '', url_certificado: '', instructor: 'Manu Rodríguez', description: 'Aprende todo lo necesario de Git de forma rápida.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'git' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="4" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -7632,7 +7644,7 @@
         <v>{ id: 3, name: 'Git + GitHub Desde Cero', category: 'Herramientas', technology: 'GitHub', url: 'https://www.udemy.com/course/aprende-git-github-practicando-con-algo-de-scrum', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 49, culminado: '2021-12-14', certificado: 'UC-a2887ba0-b933-4048-8e90-04581fd7fe77', url_certificado: 'https://www.udemy.com/certificate/UC-a2887ba0-b933-4048-8e90-04581fd7fe77', instructor: 'Jonathan Castro', description: 'Curso Git Desde Cero + Aprende GitHub con la terminal paso a paso con ejercicios.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'git','github' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="5" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -7802,7 +7814,7 @@
         <v>{ id: 4, name: 'GIT y GITHUB desde cero!', category: 'Herramientas', technology: 'GitHub', url: 'https://www.udemy.com/course/introduccion-git-github', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 90, culminado: '2021-12-10', certificado: 'S/C', url_certificado: '', instructor: 'Noelia Silva', description: 'Maneja los repositorios más actuales del mercado.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'git','github' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="6" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -7966,7 +7978,7 @@
         <v>{ id: 5, name: 'Aprende a dominar Git de cero a experto!', category: 'Herramientas', technology: 'Git', url: 'https://www.udemy.com/course/aprende-a-dominar-git-de-cero-a-experto', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 175, culminado: null, certificado: '', url_certificado: '', instructor: 'Maximiliano Burgos', description: 'Domina el mejor software de control de versiones.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'git' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="7" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -8139,7 +8151,7 @@
         <v>{ id: 6, name: 'Curso completo de Docker de cero a experto', category: 'Herramientas', technology: 'Docker', url: 'https://www.udemy.com/course/curso-completo-de-docker-de-cero-a-experto', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 0, minutos: 1020, culminado: '2021-12-30', certificado: 'UC-33aa07f4-52f4-4764-a7e8-c329febeb0bf', url_certificado: 'https://www.udemy.com/certificate/UC-33aa07f4-52f4-4764-a7e8-c329febeb0bf', instructor: 'Joan Amengual', description: '¡Conviértete en un experto en Docker con Compose, ELK, cAdvisor, Prometheus, Grafana, Kubernetes, Swarm y mucho más!', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'docker','kubernetes' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="8" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -8303,7 +8315,7 @@
         <v>{ id: 7, name: 'Master en Docker y devops de principiante a experto', category: 'Herramientas', technology: 'Docker', url: 'https://www.udemy.com/course/master-en-docker-y-devops-de-principiante-a-experto', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: false, priority: 0, minutos: 300, culminado: null, certificado: '', url_certificado: '', instructor: 'Cristian Casis', description: 'Conocer, utilizar y aprender Docker desde cero. Despliegue sus servicios de forma rápida y segura utilizando Docker.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'docker' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="9" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -8475,7 +8487,7 @@
         <v>{ id: 8, name: 'Markdown Desde Cero', category: 'Herramientas', technology: 'Markdown', url: 'https://ed.team/cursos/markdown', platform: 'EDteam', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 60, culminado: '2021-08-07', certificado: '228409101-23bffb30-c61a-4998-a82d-9a7a8c8ebfe0', url_certificado: 'https://edteam-media.s3.amazonaws.com/certificates/original/f848c8a7-28a8-4c55-af01-0eeb675bf3d2.png', instructor: 'Alvaro Felipe Chávez', description: 'Escribe código HTML limpio sin preocuparte de las etiquetas ni aprender HTML.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'edteam', logo_technologies: [ 'markdown' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="10" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -8638,7 +8650,7 @@
         <v>{ id: 9, name: 'Aprenda Markdown desde cero', category: 'Herramientas', technology: 'Markdown', url: 'https://www.udemy.com/course/aprenda-markdown-desde-cero', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 64, culminado: null, certificado: '', url_certificado: '', instructor: 'Alexander David Rodriguez Ferrer', description: 'Aprenda el lenguaje de etiquetado Markdown que facilitar la construcción de documentos en HTML 5.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'markdown' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="11" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -8801,7 +8813,7 @@
         <v>{ id: 10, name: 'VIM desde cero', category: 'Herramientas', technology: 'VIM', url: 'https://ed.team/cursos/vim', platform: 'EDteam', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 49, culminado: null, certificado: '', url_certificado: '', instructor: 'Alexys Lozada', description: 'Aprende los comandos básicos para utilizar el editor de texto más poderoso del mundo.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'edteam', logo_technologies: [ 'vim' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="12" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -8965,7 +8977,7 @@
         <v>{ id: 11, name: 'Vim, aumenta tu velocidad de desarrollo', category: 'Herramientas', technology: 'VIM', url: 'https://www.udemy.com/course/vim-aumenta-tu-velocidad-de-desarrollo', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 86, culminado: null, certificado: '', url_certificado: '', instructor: 'Nicolas Schurmann', description: 'Empieza siendo productivo con Vim en linux, windows, Mac y Unix.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'vim' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="13" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -9128,7 +9140,7 @@
         <v>{ id: 12, name: 'VIM: Mejora tu velocidad para codificar.', category: 'Herramientas', technology: 'VIM', url: 'https://www.udemy.com/course/chochy_vim', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 51, culminado: null, certificado: '', url_certificado: '', instructor: 'Jorge Salgado Miranda', description: 'Aprende a Trabajar a mayor velocidad en Cualquier IDE con ayuda de VIM y sus comandos.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'vim' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="14" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -9292,7 +9304,7 @@
         <v>{ id: 13, name: 'Curso de Blogger - Completo', category: 'Sistema de gestión de contenidos', technology: 'Blogger', url: 'https://www.youtube.com/watch?v=CcLrJQqPDPc', platform: 'YouTube', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 255, culminado: null, certificado: '', url_certificado: '', instructor: 'Yoney Gallardo', description: 'Curso completo de Blogger.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'youtube', logo_technologies: [ 'blogger' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="15" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -9456,7 +9468,7 @@
         <v>{ id: 14, name: 'Tienda Online con wordpress y Woocommerce', category: 'Sistema de gestión de contenidos', technology: 'WordPress', url: 'https://www.udemy.com/course/tienda-online-con-wordpressr-y-woocommerce', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 113, culminado: null, certificado: '', url_certificado: '', instructor: 'Roger Gómez', description: 'Tutorial básico para principiantes.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'wordpress','woocommerce' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="16" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -9620,7 +9632,7 @@
         <v>{ id: 15, name: 'Crea una página web sin programar con wordpressr y Divi', category: 'Sistema de gestión de contenidos', technology: 'WordPress', url: 'https://www.udemy.com/course/crea-una-pagina-web-sin-programar-con-wordpressr-y-divi', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 130, culminado: null, certificado: '', url_certificado: '', instructor: 'Oscar Viedma', description: 'Aprende a diseñar una página web tipo one page totalmente responsive, desde cero con wordpressr + Divi.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'wordpress' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="17" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -9784,7 +9796,7 @@
         <v>{ id: 16, name: 'Crea una Web PROFESIONAL con wordpressr y DIVI desde CERO', category: 'Sistema de gestión de contenidos', technology: 'WordPress', url: 'https://www.udemy.com/course/crea-una-web-profesional-con-wordpressr-y-divi-desde-cero', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 1080, culminado: null, certificado: '', url_certificado: '', instructor: 'José Valenzuela', description: 'Crea desde Cero a crear una web 100% Profesional con DIVI : Aprende a crear cualquier tipo de Página Web.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'wordpress' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="18" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -9947,7 +9959,7 @@
         <v>{ id: 17, name: 'Curso Magento 2.4 en la nube AWS', category: 'Sistema de gestión de contenidos', technology: 'Magento', url: 'https://www.youtube.com/playlist?list=PLyMFTgxiogL3t7n5xEeK2iDI9LaNIfITK', platform: 'YouTube', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 200, culminado: null, certificado: '', url_certificado: '', instructor: 'Aaron Ballesteros', description: 'Curso completo de Magento.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'youtube', logo_technologies: [ 'magento' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="19" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -10111,7 +10123,7 @@
         <v>{ id: 18, name: 'KUBERNETES 2021 - De NOVATO a PRO!', category: 'Herramientas', technology: 'Kubernetes', url: 'https://www.youtube.com/watch?v=DCoBcpOA7W4', platform: 'YouTube', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 93, culminado: null, certificado: '', url_certificado: '', instructor: 'Pelado Nerd', description: 'Conviertete en un profesional en Kubernetes.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'youtube', logo_technologies: [ 'kubernetes' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="20" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -10275,7 +10287,7 @@
         <v>{ id: 19, name: 'Curso de Kubernetes', category: 'Herramientas', technology: 'Kubernetes', url: 'https://www.youtube.com/playlist?list=PLrb1e2Mp6N_uJSNsV-7SqLFaBdImJsI5x', platform: 'YouTube', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 280, culminado: null, certificado: '', url_certificado: '', instructor: 'Iñigo Serrano', description: 'Curso completo de Kubernetes.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'youtube', logo_technologies: [ 'kubernetes' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="21" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -10439,7 +10451,7 @@
         <v>{ id: 20, name: 'Docker, Desarrollo práctico', category: 'Herramientas', technology: 'Docker', url: 'https://www.udemy.com/course/docker-desarrollo-practico', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: false, priority: 0, minutos: 570, culminado: null, certificado: '', url_certificado: '', instructor: 'Luis Briceño', description: 'Implementación de Dockerfile, Docker-compose, mysql, wordpressr, Node (express), mongodb y más…', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'docker' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="22" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -10603,7 +10615,7 @@
         <v>{ id: 21, name: 'Introducción a Drupal 9', category: 'Sistema de gestión de contenidos', technology: 'Drupal', url: 'https://www.udemy.com/course/introduccion-drupal-9', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 101, culminado: null, certificado: '', url_certificado: '', instructor: 'Vicente Cespedes', description: 'Curso introductorio a Drupal 9 donde aprender lo básico para adentrarse en este maravilloso CMS.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'drupal' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="23" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -10767,7 +10779,7 @@
         <v>{ id: 22, name: 'Crea sitios web con Drupal', category: 'Sistema de gestión de contenidos', technology: 'Drupal', url: 'https://www.udemy.com/course/curso-basico-de-drupal', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 118, culminado: null, certificado: '', url_certificado: '', instructor: 'Mejia Fabela', description: 'Un curso que te enseñara a usar Drupal para poder crear tu sitio web. Drupal es un poderoso administrador de contenido.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'drupal' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="24" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -10930,7 +10942,7 @@
         <v>{ id: 23, name: 'Desarrolla la Lógica de Programación con FlujoGramas', category: 'Paradigmas', technology: 'Lógica de programación', url: 'https://www.udemy.com/course/desarrolla-la-logica-de-programacion-con-flujogramas', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 120, culminado: null, certificado: '', url_certificado: '', instructor: 'Walter Coto', description: 'Aprende las Bases de la Programación, con Flujogramas. Comienza a Desarrollar tu Pensamiento de Programador desde Cero.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="25" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -11094,7 +11106,7 @@
         <v>{ id: 24, name: 'Algoritmos, desarrollo de la Lógica de Programación', category: 'Paradigmas', technology: 'Lógica de programación', url: 'https://www.udemy.com/course/algoritmos-estructuras-de-datos', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 116, culminado: null, certificado: '', url_certificado: '', instructor: 'Javier Villena', description: 'Desarrolla tu lógica de Programación creando Algoritmos.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="26" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -11258,7 +11270,7 @@
         <v>{ id: 25, name: 'Aprende Lógica de Programación (Básico)', category: 'Paradigmas', technology: 'Lógica de programación', url: 'https://www.udemy.com/course/aprende-logica-de-programacion', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 110, culminado: null, certificado: '', url_certificado: '', instructor: 'Alejandro Pérez Gabriel', description: 'Los fundamentos para un buen programador.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="27" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -11422,7 +11434,7 @@
         <v>{ id: 26, name: 'Aprende Lógica de Programación (Avanzado)', category: 'Paradigmas', technology: 'Lógica de programación', url: 'https://www.udemy.com/course/aprende-logica-de-programacion-avanzado', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 100, culminado: null, certificado: '', url_certificado: '', instructor: 'Alejandro Pérez Gabriel', description: 'Temas intermedios y avanzados de lógica para un buen programador.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="28" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -11586,7 +11598,7 @@
         <v>{ id: 27, name: 'Curso de Fundamentos y Lógica de Programación -Bootcamp 2021', category: 'Paradigmas', technology: 'Lógica de programación', url: 'https://www.udemy.com/course/fundamentos-programacion-curso', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 450, culminado: null, certificado: '', url_certificado: '', instructor: 'Jeovani Martínez', description: 'Aprende las bases y la lógica de la programación con el mejor curso, y prepárate para aprender cualquier lenguaje.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="29" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -11750,7 +11762,7 @@
         <v>{ id: 28, name: 'Lógica Programación: Aprende Programar en Cualquier Lenguaje', category: 'Paradigmas', technology: 'Lógica de programación', url: 'https://www.udemy.com/course/logica-programacion-aprende-programar-en-cualquier-lenguaje', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 160, culminado: null, certificado: '', url_certificado: '', instructor: 'Sayyab Tariq Awan', description: 'Un curso muy básico para aprender a programar en cualquier lenguaje: Java, C++, javascript, python, SQL, HTML, Swift etc.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="30" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -11914,7 +11926,7 @@
         <v>{ id: 29, name: 'Curso POO y Java Básico', category: 'Paradigmas', technology: 'POO', url: 'https://www.udemy.com/course/curso-poo-y-java-basico-1', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 89, culminado: null, certificado: '', url_certificado: '', instructor: 'Flores Aguilar', description: 'Curso de conceptos básicos de POO y Java.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'java' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="31" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -12078,7 +12090,7 @@
         <v>{ id: 30, name: 'CURSO de php &amp; MVC: Mi primer SISTEMA [php, MVC, POO, mysql]', category: 'Paradigmas', technology: 'POO', url: 'https://www.udemy.com/course/mi-primer-sistema-php-mvc-mysql', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 111, culminado: null, certificado: '', url_certificado: '', instructor: 'Carlos Alfaro', description: 'CURSO de php, MVC, POO &amp; mysql: Aprende a PROGRAMAR un SISTEMA web [php, MVC, POO, mysql &amp; ajax]', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'php','mysql' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="32" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -12242,7 +12254,7 @@
         <v>{ id: 31, name: 'Introducción a MVC con Net 5', category: 'Paradigmas', technology: 'MVC', url: 'https://www.udemy.com/course/introduccion-a-mvc-con-net-5', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 79, culminado: null, certificado: '', url_certificado: '', instructor: 'Misael Cazarez', description: 'Creación de CRUD en MVC.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="33" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -12412,7 +12424,7 @@
         <v>{ id: 32, name: 'Aprende a diseñar una API RESTFul correctamente', category: 'Paradigmas', technology: 'API RESTful', url: 'https://www.udemy.com/course/aprende-a-disenar-una-api-restful-correctamente', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 68, culminado: '2021-09-26', certificado: 'S/C', url_certificado: '', instructor: 'Eduardo Patiño', description: 'Fortalece tus bases sobre el diseño antes de programar.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'apirestful' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="34" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -12588,7 +12600,7 @@
         <v>{ id: 33, name: 'API RESTful con laravel: Guía Definitiva', category: 'Paradigmas', technology: 'API RESTful', url: 'https://www.udemy.com/course/api-restful-con-laravel-php-homestead-passport', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 0, minutos: 900, culminado: '2022-03-16', certificado: 'UC-777de1a6-3ed2-4a9f-a30c-78a0037ad1cd', url_certificado: 'https://www.udemy.com/certificate/UC-777de1a6-3ed2-4a9f-a30c-78a0037ad1cd', instructor: 'Juan David Meza González', description: 'Crea la API RESTful de un sistema de mercado con laravel y domina características complejas de las API con laravel', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'apirestful','laravel' ], mostrar: false, repositorio: 'https://github.com/petrix12/api_restful_2021', nota: '' },</v>
       </c>
     </row>
-    <row r="35" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -12761,7 +12773,7 @@
         <v>{ id: 34, name: 'Aprende a crear una API RESTful con laravel', category: 'Paradigmas', technology: 'API RESTful', url: 'https://codersfree.com/cursos/aprende-a-crear-una-api-restful-con-laravel', platform: 'Coders Free', costo: 9.99, money: 'USD', comprado: true, priority: 0, minutos: 540, culminado: '2021-09-23', certificado: 'UC-253cc4d8-67d5-4b6c-b6b5-ffea89ea0bf4', url_certificado: 'https://www.udemy.com/certificate/UC-253cc4d8-67d5-4b6c-b6b5-ffea89ea0bf4', instructor: 'Victor Arana Flores', description: 'En este curso aprenderás a crear una API RESTful con el framework laravel.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'coders_free', logo_technologies: [ 'apirestful' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="36" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -12925,7 +12937,7 @@
         <v>{ id: 35, name: 'React.js', category: 'Frameworks de JavaScript', technology: 'React JS', url: 'https://www.udemy.com/course/react-js-curso', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 93, culminado: null, certificado: '', url_certificado: '', instructor: 'Pablo Monteserín', description: 'Aprende en un tiempo record a crear aplicaciones con React.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'reactjs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="37" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -13089,7 +13101,7 @@
         <v>{ id: 36, name: 'Crea APIREST fácilmente con python, php, laravel o nodejs', category: 'Paradigmas', technology: 'API RESTful', url: 'https://www.udemy.com/course/crea-api-rest-facilmente-con-python-php-laravel-y-nodejs', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 1, minutos: 240, culminado: null, certificado: '', url_certificado: '', instructor: 'Davis Anderson Bastidas Vicente', description: 'API REST python, php, laravel o nodejs, Consumo con POSTMAN.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'apirestful','python','php','laravel','nodejs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="38" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -13253,7 +13265,7 @@
         <v>{ id: 37, name: 'Curso Crea una REST API desde Cero con nodejs y AdonisJS', category: 'Paradigmas', technology: 'API RESTful', url: 'https://www.udemy.com/course/curso-crea-una-rest-api-desde-cero-con-nodejs-y-adonisjs', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 240, culminado: null, certificado: '', url_certificado: '', instructor: 'Marcos Guerrini', description: 'Aprende a utilizar uno de los frameworks más potentes de nodejs.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'apirestful','nodejs','adonisjs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="39" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -13417,7 +13429,7 @@
         <v>{ id: 38, name: 'Servicios Web API y WCF crea y consume en App Web y Móvil', category: 'Paradigmas', technology: 'API RESTful', url: 'https://www.udemy.com/course/ccrea-servicios-wcf-y-web-api-y-consume-en-app-web-y-movil', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 570, culminado: null, certificado: '', url_certificado: '', instructor: 'Licito Hurol', description: 'Aprende a crear servicios WCF y Web API y a consumirlos desde otro aplicación o desde el navegador.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'apirestful' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="40" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -13581,7 +13593,7 @@
         <v>{ id: 39, name: 'Node.js - Creando API con express y mongodb (Incl. Deno)', category: 'Paradigmas', technology: 'API RESTful', url: 'https://www.udemy.com/course/nodejs-guia-desde-cero', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 1, minutos: 750, culminado: null, certificado: '', url_certificado: '', instructor: 'Grover Vásquez', description: 'Node.js, API REST, express, mongodb, JWT, Autenticación, PostMan y Despliegue en Producción - Introducción a Deno.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'apirestful','nodejs','express','mongo' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="41" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -13744,7 +13756,7 @@
         <v>{ id: 40, name: 'Fundamentos de Programación - Algoritmos y javascript', category: 'Paradigmas', technology: 'Lógica de programación', url: 'https://www.udemy.com/course/fundamentos-de-programacion-algoritmos-y-javascript', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 53, culminado: null, certificado: '', url_certificado: '', instructor: 'Roger Gómez', description: 'Curso muy básico introductorio a la programación', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'javascript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="42" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>41</v>
       </c>
@@ -13917,7 +13929,7 @@
         <v>{ id: 41, name: 'Programación desde cero', category: 'Paradigmas', technology: 'Lógica de programación', url: 'https://ed.team/cursos/programacion', platform: 'EDteam', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 300, culminado: '2021-08-10', certificado: '228409205-3d369290-b9d0-4131-b346-b316d9939c89', url_certificado: 'https://edteam-media.s3.amazonaws.com/certificates/original/5df5fc3d-148a-46d4-99bb-d8ef62e385d6.png', instructor: 'Alvaro Felipe Chávez', description: 'Programar no se trata de código, se trata de lógica. Este curso te enseña la lógica que te permitirá dominar cualquier lenguaje.', url_aux: '', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'edteam', logo_technologies: [ 'javascript','python' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="43" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>42</v>
       </c>
@@ -14090,7 +14102,7 @@
         <v>{ id: 42, name: 'Curso de Introducción al Desarrollo Web: HTML y css (1/2)', category: 'Front-end', technology: 'HTML', url: 'https://learndigital.withgoogle.com/activate/course/web-development-I', platform: 'Google Activate', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 2400, culminado: '2020-05-25', certificado: '7DJ 77F R2R', url_certificado: 'https://learndigital.withgoogle.com/activate/validate-certificate-code', instructor: 'Sergio Luján Mora', description: 'Aprende a crear tus propias páginas web profesionales adaptables a distintos dispositivos de la mano de la Universidad de Alicante.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'google', logo_technologies: [ 'html5' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="44" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>43</v>
       </c>
@@ -14263,7 +14275,7 @@
         <v>{ id: 43, name: 'Curso de Introducción al Desarrollo Web: HTML y css (2/2)', category: 'Front-end', technology: 'css', url: 'https://learndigital.withgoogle.com/activate/course/web-development-II', platform: 'Google Activate', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 2400, culminado: '2020-06-05', certificado: 'QNK V22 H93', url_certificado: 'https://learndigital.withgoogle.com/activate/validate-certificate-code', instructor: 'Sergio Luján Mora', description: 'Aprende a crear tus propias páginas web profesionales adaptables a distintos dispositivos de la mano de la Universidad de Alicante.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'google', logo_technologies: [ 'css','html5' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="45" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -14427,7 +14439,7 @@
         <v>{ id: 44, name: 'Curso de css-todo lo que necesitas saber sobre css y css3', category: 'Front-end', technology: 'css', url: 'https://www.udemy.com/course/curso-de-css-introduccion-a-las-hojas-de-estilos-en-cascada', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 510, culminado: null, certificado: '', url_certificado: '', instructor: 'Andrés Sosa Arevalo', description: 'Aprende a agregar estilos a tus plantillas Html desde cero, contiene muchos ejercicios y se agregaran nuevos.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'css' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="46" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -14591,7 +14603,7 @@
         <v>{ id: 45, name: 'Curso javascript desde cero', category: 'Front-end', technology: 'javascript', url: 'https://www.youtube.com/playlist?list=PLZ2ovOgdI-kXnDbWdaJK7GA1GvKGNMl6B', platform: 'YouTube', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 300, culminado: null, certificado: '', url_certificado: '', instructor: 'Victor Arana Flores', description: 'Curso completo de javascript.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'youtube', logo_technologies: [ 'javascript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="47" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -14755,7 +14767,7 @@
         <v>{ id: 46, name: 'Universidad javascript 2021 - De Cero a Experto javascript!', category: 'Front-end', technology: 'javascript', url: 'https://www.udemy.com/course/universidad-javascript-angular-react-vue-typescript-html-css-bootstrap', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 2160, culminado: null, certificado: '', url_certificado: '', instructor: 'Ubaldo Acosta', description: '[Actualizado 2021] - Programación Orientada a Objetos, Funciones Flecha, Callback, Promesas, Async, Await, DOM y más!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'javascript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="48" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -14918,7 +14930,7 @@
         <v>{ id: 47, name: 'Curso de css3, Flexbox y css Grid Layout | Básico y rápido', category: 'Front-end', technology: 'css', url: 'https://www.udemy.com/course/curso-de-css3-flexbox-y-css-grid-layout-basico', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 57, culminado: null, certificado: '', url_certificado: '', instructor: 'Víctor Robles', description: 'Aprende css 3, css Flexbox y Grid Layout y da tus primeros pasos en la maquetación web. Dale estilos a tus páginas web.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'css' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="49" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -15081,7 +15093,7 @@
         <v>{ id: 48, name: 'FLEXBOX (css3) | Aprende FLEXBOX DESDE CERO', category: 'Front-end', technology: 'css', url: 'https://www.udemy.com/course/cursoflexbox', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 57, culminado: null, certificado: '', url_certificado: '', instructor: 'Jordan Alexander', description: 'Aprende y Entiende Flexbox, El módulo flexible más popular de css.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'css' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="50" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -15245,7 +15257,7 @@
         <v>{ id: 49, name: 'Crea una página web moderna con HTML css Y javascript', category: 'Front-end', technology: 'Estándares Front-end', url: 'https://www.udemy.com/course/crea-una-pagina-web-moderna-con-html-css-y-javascript', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 79, culminado: null, certificado: '', url_certificado: '', instructor: 'Jordan Alexander', description: 'Aprende a crear una página web con html5 css3 y Javacript, [Adaptable a dispositivos móviles]', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'html5','css','javascript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="51" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -15408,7 +15420,7 @@
         <v>{ id: 50, name: 'Crea una LANDING PAGE moderna con HTML css Y javascript', category: 'Front-end', technology: 'Estándares Front-end', url: 'https://www.udemy.com/course/crea-una-landing-page-moderna-con-html-css-y-javascript', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 51, culminado: null, certificado: '', url_certificado: '', instructor: 'Jordan Alexander', description: 'Aprende a crear una landing page moderna desde 0 con html5 css3 y JS (javascript) con animaciones hechas en css3.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'html5','css','javascript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="52" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -15572,7 +15584,7 @@
         <v>{ id: 51, name: 'Crea una página web profesional con HTML css y javascript', category: 'Front-end', technology: 'Estándares Front-end', url: 'https://www.udemy.com/course/crea-una-pagina-web-profesional-con-html-css-y-javascript', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 163, culminado: null, certificado: '', url_certificado: '', instructor: 'Jordan Alexander', description: 'En este curso aprenderás a crear una página web desde 0 con HTML css y javascript además aprenderás a subirla a internet.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'html5','css','javascript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="53" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -15735,7 +15747,7 @@
         <v>{ id: 52, name: 'Curso de Desarrollo Web con HTML, css y javascript | Básico', category: 'Front-end', technology: 'Estándares Front-end', url: 'https://www.udemy.com/course/curso-de-desarrollo-web-con-html-css-y-javascript', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 55, culminado: null, certificado: '', url_certificado: '', instructor: 'Víctor Robles', description: 'Aprende HTML, css y javascript desde cero y da tus primeros pasos en el desarrollo web. Crea tu primera web paso a paso.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'html5','css','javascript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="54" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -15898,7 +15910,7 @@
         <v>{ id: 53, name: 'Diseño Web - Aprende creando un sitio web paso a paso', category: 'Front-end', technology: 'Estándares Front-end', url: 'https://www.udemy.com/course/diseno-web-aprende-creando-un-sitio-web', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 55, culminado: null, certificado: '', url_certificado: '', instructor: 'Grover Vásquez', description: 'Aprende a crear un sitio web desde cero con html5, css3 y jQuery, y que pueda ser visto en cualquier dispositivo.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'html5','css','javascript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="55" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -16062,7 +16074,7 @@
         <v>{ id: 54, name: 'Universidad Desarrollo Web - FrontEnd Web Developer!', category: 'Front-end', technology: 'Estándares Front-end', url: 'https://www.udemy.com/course/universidad-desarrollo-web-moderno-html-css-javascript-html5-css3', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 1830, culminado: null, certificado: '', url_certificado: '', instructor: 'Ubaldo Acosta', description: 'El mejor curso para aprender a crear aplicaciones Web Modernas con HTML, css y javascript. Serás un FrontEnd Developer!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'html5','css','javascript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="56" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -16226,7 +16238,7 @@
         <v>{ id: 55, name: 'Aprende TypeScript desde cero', category: 'Front-end', technology: 'TypeScript', url: 'https://www.udemy.com/course/aprende-typescript-desde-cero', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 420, culminado: null, certificado: '', url_certificado: '', instructor: 'JAP Software', description: 'Curso de iniciación a TypeScript.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'typescript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="57" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -16390,7 +16402,7 @@
         <v>{ id: 56, name: 'Aprende Typescript de 0 a 100', category: 'Front-end', technology: 'TypeScript', url: 'https://www.udemy.com/course/typescript-2020', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 210, culminado: null, certificado: '', url_certificado: '', instructor: 'Manuel Muñoz', description: 'Aprende Typescript en poco tiempo y de forma sencilla.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'typescript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="58" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -16554,7 +16566,7 @@
         <v>{ id: 57, name: 'La biblia perdida de bootstrap 4', category: 'Frameworks de css', technology: 'bootstrap', url: 'https://www.udemy.com/course/curso-la-biblia-perdida-de-bootstrap-4', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 568, culminado: null, certificado: '', url_certificado: '', instructor: 'Erick Mines', description: 'Los secretos de bootstrap por fin te serán revelados. Acompáñame a descubrir el verdadero poder que esconde bootstrap 4.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'bootstrap' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="59" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -16718,7 +16730,7 @@
         <v>{ id: 58, name: 'Desarrollo Web con HMTL, css y bootstrap 4! Curso desde cero', category: 'Frameworks de css', technology: 'bootstrap', url: 'https://www.udemy.com/course/curso-html5-css3', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 163, culminado: null, certificado: '', url_certificado: '', instructor: 'Ignacio Gutiérrez ', description: 'Curso de HTML, css y bootstrap 4 para principiantes, comienza a crear tus propios diseños web sin conocimientos previos!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'bootstrap','html5','css' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="60" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -16881,7 +16893,7 @@
         <v>{ id: 59, name: 'materialize css - Tutorial Español', category: 'Frameworks de css', technology: 'materialize', url: 'https://www.youtube.com/playlist?list=PLPl81lqbj-4J2Lbx1_qp7Yzo7wvjYiQ4E', platform: 'YouTube', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 300, culminado: null, certificado: '', url_certificado: '', instructor: 'Ignacio Gutiérrez ', description: 'Curso completo del materialize.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'youtube', logo_technologies: [ 'materialize' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="61" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>60</v>
       </c>
@@ -17045,7 +17057,7 @@
         <v>{ id: 60, name: 'Curso Tailwind desde cero', category: 'Frameworks de css', technology: 'Tailwind', url: 'https://codersfree.com/cursos/curso-tailwind-desde-cero', platform: 'Coders Free', costo: 0, money: 'USD', comprado: true, priority: 1, minutos: 180, culminado: null, certificado: '', url_certificado: '', instructor: 'Victor Arana Flores', description: 'En este nuevo curso aprenderemos a como trabajar con el framework Tailwind css dentro de un framework más grande como lo es laravel.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'coders_free', logo_technologies: [ 'tailwindcss' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="62" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -17209,7 +17221,7 @@
         <v>{ id: 61, name: 'Tailwind css - Fundamentos desde 0! ¿Mejor que bootstrap 4?', category: 'Frameworks de css', technology: 'Tailwind', url: 'https://www.udemy.com/course/tailwindcss', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 110, culminado: null, certificado: '', url_certificado: '', instructor: 'Ignacio Gutiérrez ', description: 'Trabaja con Tailwind css de una manera sencilla, desde 0 y paso a paso, curso introductorio para aplicar sus clases css!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'tailwindcss' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="63" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -17373,7 +17385,7 @@
         <v>{ id: 62, name: 'Curso express de TAILWIND css de cero a EXPERTO', category: 'Frameworks de css', technology: 'Tailwind', url: 'https://www.udemy.com/course/curso-express-de-tailwindcss-de-cero-a-experto', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 92, culminado: null, certificado: '', url_certificado: '', instructor: 'Marcos Rivas', description: 'Aprende los conceptos de Tailwindcss creando un sitio web responsivo.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'tailwindcss' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="64" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -17537,7 +17549,7 @@
         <v>{ id: 63, name: 'Introducción a Figma', category: 'Herramientas', technology: 'Figma', url: 'https://www.udemy.com/course/figma-diseno-de-prototipos-desde-cero', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 118, culminado: null, certificado: '', url_certificado: '', instructor: 'Javier Cañas', description: 'Conoce y aprende desde cero cómo utilizar Figma y las herramientas para diseñar interfaces con Figma.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'figma' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="65" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -17700,7 +17712,7 @@
         <v>{ id: 64, name: 'Curso Bulma css', category: 'Frameworks de css', technology: 'Bulma', url: 'https://www.youtube.com/playlist?list=PLvKwKSrP7HoAbR5bXjwb4h5f2xjVxqdEe', platform: 'YouTube', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 500, culminado: null, certificado: '', url_certificado: '', instructor: 'Designlopers', description: 'Curso completo de Bulma css.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'youtube', logo_technologies: [ 'bulma' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="66" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -17863,7 +17875,7 @@
         <v>{ id: 65, name: 'Primeros pasos con Vue.js | Vue en ejercicios', category: 'Frameworks de JavaScript', technology: 'Vue JS', url: 'https://www.udemy.com/course/draft/2219980/learn/lecture/13667902?start=0#overview', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 294, culminado: null, certificado: '', url_certificado: '', instructor: 'Andrés Cruz Yoris', description: 'En este mini curso te voy a explicar cómo puedes trabajar con el framework javascript Vue.js de la manera más fácil.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'vuejs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="67" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -18027,7 +18039,7 @@
         <v>{ id: 66, name: 'Vue JS (2 y 3) - Crea Aplicaciones Web Modernas con Vue', category: 'Frameworks de JavaScript', technology: 'Vue JS', url: 'https://www.udemy.com/course/vue-js-2-para-principiantes', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 840, culminado: null, certificado: '', url_certificado: '', instructor: 'Grover Vásquez', description: 'Todo sobre Vue JS 2 y 3, Bindings, Directivas, Vue-CLI, Componentes, Formularios, Vue-Router, Composition API y Vuex.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'vuejs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="68" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A68" s="7">
         <v>67</v>
       </c>
@@ -18191,7 +18203,7 @@
         <v>{ id: 67, name: 'Vue 3 Desde Cero', category: 'Frameworks de JavaScript', technology: 'Vue JS', url: 'https://www.udemy.com/course/vue-3-desde-cero', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 1, minutos: 1890, culminado: null, certificado: '', url_certificado: '', instructor: 'Yirsis Serrano', description: 'Aprenderás Vue con la Options API y la nueva Composition API, Integración con PUG, sass y TypeScript, PWA y mucho mas.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'vuejs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="69" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -18355,7 +18367,7 @@
         <v>{ id: 68, name: 'Curso Super Básico de Vue.js', category: 'Frameworks de JavaScript', technology: 'Vue JS', url: 'https://www.udemy.com/course/curso-basico-de-vue', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 111, culminado: null, certificado: '', url_certificado: '', instructor: 'Cristhian Santa Cruz', description: 'Curso básico de Vue.js Framework de javascript.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'vuejs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="70" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -18519,7 +18531,7 @@
         <v>{ id: 69, name: 'Primeros pasos en Vue 3 Composition API', category: 'Frameworks de JavaScript', technology: 'Vue JS', url: 'https://www.udemy.com/course/primeros-pasos-en-vue-3-composition-api', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 82, culminado: null, certificado: '', url_certificado: '', instructor: 'Cursos de desarrollo web', description: 'Conoce las bases de la nueva API de Vue 3.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'vuejs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="71" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A71" s="7">
         <v>70</v>
       </c>
@@ -18683,7 +18695,7 @@
         <v>{ id: 70, name: 'Vue.js: De cero a experto', category: 'Frameworks de JavaScript', technology: 'Vue JS', url: 'https://www.udemy.com/course/vuejs-fh', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 1, minutos: 2580, culminado: null, certificado: '', url_certificado: '', instructor: 'Fernando Herrera', description: 'Vuex, unit test, composition api, options api, autenticación, composables, deployment, file structure, lazy load, y más.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'vuejs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="72" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -18856,7 +18868,7 @@
         <v>{ id: 71, name: 'Aprende Vue 3 desde cero + inertia', category: 'Frameworks de JavaScript', technology: 'Vue JS', url: 'https://codersfree.com/cursos/aprende-vue-3-desde-cero-mas-inertia', platform: 'Coders Free', costo: 9.99, money: 'USD', comprado: true, priority: 0, minutos: 918, culminado: '2022-03-14', certificado: 'S/C', url_certificado: '', instructor: 'Victor Arana Flores', description: 'En este curso aprenderás las bases del desarrollo web con Inertia.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'coders_free', logo_technologies: [ 'vuejs','laravel' ], mostrar: true, repositorio: 'https://github.com/petrix12/inertia2022', nota: '' },</v>
       </c>
     </row>
-    <row r="73" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -19020,7 +19032,7 @@
         <v>{ id: 72, name: '60+ Herramientas de desarrollo y diseño web', category: 'Herramientas', technology: 'General', url: 'https://www.udemy.com/course/recursos-web-plugins-y-utilidades', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 489, culminado: null, certificado: '', url_certificado: '', instructor: 'Fernando Herrera', description: 'Una completa colección de recursos que debes tener y conocer, totalmente gratuitos.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="74" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>73</v>
       </c>
@@ -19193,7 +19205,7 @@
         <v>{ id: 73, name: 'Crea un CRUD con laravel, Sweetalert2, Toastr, vuejs y Axios', category: 'Frameworks de JavaScript', technology: 'Vue JS', url: 'https://www.udemy.com/course/crea-un-crud-con-laravel-sweetalert2-toastr-vuejs-y-axios', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 150, culminado: '2021-10-27', certificado: 'UC-0e1d1558-902d-46e0-bad9-082faa58cb7b', url_certificado: 'https://www.udemy.com/certificate/UC-0e1d1558-902d-46e0-bad9-082faa58cb7b/', instructor: 'Jhonatan Fernández', description: 'En este curso aprenderás a crear un CRUD con estas tecnologías.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'laravel','sweetalert2','vuejs','axios' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="75" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -19358,7 +19370,7 @@
         <v>{ id: 74, name: 'Aprende Jquery para implementar tus aplicaciones web', category: 'Frameworks de JavaScript', technology: 'jQuery', url: 'https://www.udemy.com/course/aprende-jquery-para-implementar-tus-aplicaciones-web', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 178, culminado: null, certificado: '', url_certificado: '', instructor: 'Carlos Blanco Gómez', description: 'Aprenderás todos lo conocimientos necesarios para agregar jquery a tus páginas web y hacerlas más dinámicas.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'jquery' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="76" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A76" s="6">
         <v>75</v>
       </c>
@@ -19527,7 +19539,7 @@
         <v>{ id: 75, name: 'Vue 3 - Composition API, Vuex, API Rest - Rick And Morty', category: 'Frameworks de JavaScript', technology: 'Vue JS', url: 'https://www.udemy.com/course/vue-3-composition-api-vuex-api-rest-rick-and-morty', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 35, culminado: '2021-10-16', certificado: 'S/C', url_certificado: '', instructor: 'Carlos Córdova', description: 'Crea un app web de Rick And Morty para tu portafolio utilizando Vue 3 - Vuex.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'vuejs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="77" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -19691,7 +19703,7 @@
         <v>{ id: 76, name: 'jQuery y ajax Desde Cero - La Guía Definitiva', category: 'Frameworks de JavaScript', technology: 'jQuery', url: 'https://www.udemy.com/course/curso-de-jquery', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 159, culminado: null, certificado: '', url_certificado: '', instructor: 'Pablo Farias Navarro', description: 'Crea sitios web y apps de html5 dinámicos, interactivos y con animaciones.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'jquery','ajax' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="78" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -19855,7 +19867,7 @@
         <v>{ id: 77, name: 'Universidad angular - De Cero a Experto en angular!', category: 'Frameworks de JavaScript', technology: 'angular', url: 'https://www.udemy.com/course/angular-de-cero-a-experto-angular-2-framework-javascript-html-css', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 3090, culminado: null, certificado: '', url_certificado: '', instructor: 'Ubaldo Acosta', description: 'Domina angular 11 y crea aplicaciones web del mundo real con TypeScript, firebase, Firestore, JWT y más!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'angular' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="79" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -20019,7 +20031,7 @@
         <v>{ id: 78, name: 'Compodoc: Crea documentación en proyectos angular/Ionic/TS', category: 'Frameworks de JavaScript', technology: 'angular', url: 'https://www.udemy.com/course/compodoc-crea-documentacion-en-angular-ionic', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 184, culminado: null, certificado: '', url_certificado: '', instructor: 'Anartz Mugika Ledo', description: 'Crear documentación de calidad y MUY fácil de mantener con Compodoc para proyectos de angular 2+ / Ionic 2+ / Typescript.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'angular' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="80" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -20183,7 +20195,7 @@
         <v>{ id: 79, name: 'CRUD angular - Node - MEAN', category: 'Stack', technology: 'MEAN', url: 'https://www.udemy.com/course/crud-productos-stack-mean', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 118, culminado: null, certificado: '', url_certificado: '', instructor: 'Tomas Ruiz Diaz', description: 'Aprende a desarrollar un CRUD completo con el Stack MEAN (Mongo, express, angular y Node) desde cero.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'mongo','express','angular','nodejs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="81" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -20347,7 +20359,7 @@
         <v>{ id: 80, name: 'App Empleados con angular 11 y firebase', category: 'Frameworks de JavaScript', technology: 'angular', url: 'https://www.udemy.com/course/app-empleado-angular-firebase', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 119, culminado: null, certificado: '', url_certificado: '', instructor: 'Tomas Ruiz Diaz', description: 'Crearemos un CRUD en angular, utilizaremos como BackEnd firebase, Firestore y deployaremos el proyecto.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'angular','firebase' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="82" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -20511,7 +20523,7 @@
         <v>{ id: 81, name: 'angular: Convierte cualquier template HTML en una WebAPP', category: 'Frameworks de JavaScript', technology: 'angular', url: 'https://www.udemy.com/course/html-hacia-angular', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 208, culminado: null, certificado: '', url_certificado: '', instructor: 'Fernando Herrera', description: '¿Quieres aprender a crear un sitio web dinámico con angular, firebase y GitHub Pages? Estas en el lugar correcto.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'angular','html5' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="83" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -20675,7 +20687,7 @@
         <v>{ id: 82, name: 'CRUD angular + NET Core + Entity Framework Core + mysql', category: 'Frameworks de JavaScript', technology: 'angular', url: 'https://www.udemy.com/course/crud-angular-9-net-core-entity-framework-core-mysql', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 62, culminado: null, certificado: '', url_certificado: '', instructor: 'Tomas Ruiz Diaz', description: 'Desarrollo frontend con angular 9, backend NET Core 3, Entity Framework Core 3 y mysql!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'angular','net_core' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="84" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -20839,7 +20851,7 @@
         <v>{ id: 83, name: 'angular - NET Core - Aplicacion de Preguntas y Respuestas', category: 'Frameworks de JavaScript', technology: 'angular', url: 'https://www.udemy.com/course/angular-net-core-aplicacion-de-preguntas-y-respuestas', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 900, culminado: null, certificado: '', url_certificado: '', instructor: 'Tomas Ruiz Diaz', description: 'Aprende a desarrollar aplicaciones modernas con angular 10 y .NET Core 3 desde cero!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'angular','mysql' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="85" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -21003,7 +21015,7 @@
         <v>{ id: 84, name: 'Fundamentos de angular', category: 'Frameworks de JavaScript', technology: 'angular', url: 'https://www.udemy.com/course/fundamentos-de-angular-12', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 240, culminado: null, certificado: '', url_certificado: '', instructor: 'Alejandro Toro Ossaba', description: 'Aprende los conceptos necesarios para comenzar a desarrollar aplicaciones con angular.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'angular','mysql' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="86" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A86" s="7">
         <v>85</v>
       </c>
@@ -21167,7 +21179,7 @@
         <v>{ id: 85, name: 'React: De cero a experto ( Hooks y MERN )', category: 'Stack', technology: 'MERN', url: 'https://www.udemy.com/course/react-cero-experto', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 1, minutos: 2940, culminado: null, certificado: '', url_certificado: '', instructor: 'Fernando Herrera', description: 'Context API, MERN, Hooks, Firestore, JWT, Testing, Autenticaciones, Despliegues, CRUD, Logs, sass, Multiple Routers…', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'mongo','express','reactjs','nodejs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="87" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -21330,7 +21342,7 @@
         <v>{ id: 86, name: 'Full-Stack CRUD con React JS, ASP.NET Core y SQL Server', category: 'Frameworks de JavaScript', technology: 'React JS', url: 'https://www.udemy.com/course/full-stack-crud-con-react-js-aspnet-core-y-sql-server', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 49, culminado: null, certificado: '', url_certificado: '', instructor: 'Arturo Borja', description: 'Creando y conectando un CRUD con API Rest utilizando React JS y ASP.NET Core.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'reactjs','net_core','sqlserver' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="88" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -21493,7 +21505,7 @@
         <v>{ id: 87, name: 'Full-Stack CRUD con php, mysql, API Rest, PDO y React JS', category: 'Frameworks de JavaScript', technology: 'React JS', url: 'https://www.udemy.com/course/full-stack-php-y-react-js', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 49, culminado: null, certificado: '', url_certificado: '', instructor: 'Arturo Borja', description: 'Creando y conectando un CRUD con API Rest utilizando React JS y php.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'php','mysql','apirestful','reactjs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="89" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -21657,7 +21669,7 @@
         <v>{ id: 88, name: 'Aprende React + firebase | 2021 Actualizado', category: 'Frameworks de JavaScript', technology: 'React JS', url: 'https://www.udemy.com/course/aprende-react-firebase-2021-actualizado', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 390, culminado: null, certificado: '', url_certificado: '', instructor: 'Manuel Muñoz', description: 'javascript + React + firebase todo lo que necesitas saber.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'reactjs','firebase' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="90" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
         <v>89</v>
       </c>
@@ -21821,7 +21833,7 @@
         <v>{ id: 89, name: 'React Desde Cero', category: 'Frameworks de JavaScript', technology: 'React JS', url: 'https://www.udemy.com/course/react-desde-cero-pwa', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 2190, culminado: null, certificado: '', url_certificado: '', instructor: 'Yirsis Serrano', description: 'Aprenderás React de la mano con PWA, React Hooks, firebase, React Router, Optimizaciones, Redux, sass y muchos temas mas.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'reactjs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="91" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A91" s="6">
         <v>90</v>
       </c>
@@ -22163,7 +22175,7 @@
         <v>{ id: 91, name: 'Curso de laravel 5 y Vue.js [desde cero] - Español', category: 'Frameworks de back-end', technology: 'Laravel', url: 'https://www.youtube.com/playlist?list=PLPl81lqbj-4KHPEGngoy5PSjjxcwnpCdb', platform: 'YouTube', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 265, culminado: '2020-08-20', certificado: 'S/C', url_certificado: '', instructor: 'Ignacio Gutiérrez ', description: 'Si tu idea es trabajar con php de forma segura y realizar aplicaciones web a la velocidad de la luz, te informo que laravel 5 cuenta con estas maravillas.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'youtube', logo_technologies: [ 'laravel' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="93" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
         <v>92</v>
       </c>
@@ -22333,7 +22345,7 @@
         <v>{ id: 92, name: 'Curso de Vue JS - Tutorial en Español [Desde Cero]', category: 'Frameworks de JavaScript', technology: 'Vue JS', url: 'https://www.youtube.com/playlist?list=PLPl81lqbj-4J-gfAERGDCdOQtVgRhSvIT', platform: 'YouTube', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 900, culminado: '2020-08-26', certificado: 'S/C', url_certificado: '', instructor: 'Ignacio Gutiérrez ', description: 'Aprende a trabajar con este hermoso framework de javascript que es realmente poderoso.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'youtube', logo_technologies: [ 'vuejs' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="94" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A94" s="6">
         <v>93</v>
       </c>
@@ -22672,7 +22684,7 @@
         <v>{ id: 94, name: 'Introducción a laravel 5 - Primeros pasos con este framework', category: 'Frameworks de back-end', technology: 'Laravel', url: 'https://www.udemy.com/course/introduccion-a-laravel-5-primeros-pasos-framework-php', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 60, culminado: '2020-10-09', certificado: 'S/C', url_certificado: '', instructor: 'Víctor Robles', description: 'Aprende las bases de la laravel 5 desde cero, el framework para php más popular de la actualidad. Introducción básica.', url_aux: '', calificacion: 'Bueno', actualizado: false, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'laravel' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="96" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A96" s="6">
         <v>95</v>
       </c>
@@ -22841,7 +22853,7 @@
         <v>{ id: 95, name: 'React JS - Curso de introducción desde cero y primeros pasos', category: 'Frameworks de JavaScript', technology: 'React JS', url: 'https://www.udemy.com/course/react-js-curso-de-introduccion-desde-cero-y-primeros-pasos', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 60, culminado: '2020-10-10', certificado: 'S/C', url_certificado: '', instructor: 'Víctor Robles', description: 'Aprende los fundamentos básicos de React desde cero y paso a paso con Víctor Robles. Instalación, Componentes, JSX y más.', url_aux: '', calificacion: 'Bueno', actualizado: false, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'reactjs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="97" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A97" s="10">
         <v>96</v>
       </c>
@@ -23005,7 +23017,7 @@
         <v>{ id: 96, name: 'React - La Guía Completa: Hooks Context Redux MERN +15 Apps', category: 'Frameworks de JavaScript', technology: 'React JS', url: 'https://www.udemy.com/course/react-de-principiante-a-experto-creando-mas-de-10-aplicaciones', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: false, priority: 0, minutos: 3488, culminado: null, certificado: '', url_certificado: '', instructor: 'Juan Pablo De La Torre Valdez', description: 'Incluye React Hooks Gatsby GraphQL Firestore Redux Context MERN Next.js Styled Components Testing Cypress +15 PROYECTOS!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'mongo','express','reactjs','nodejs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="98" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A98" s="5">
         <v>97</v>
       </c>
@@ -23169,7 +23181,7 @@
         <v>{ id: 97, name: 'Curso básico de sass, css3, html5 y jQuery creando un sitio', category: 'Preprocesadores de css', technology: 'sass', url: 'https://www.udemy.com/course/aprende-html5-sass-y-jquery-creando-un-sitio-desde-cero', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 431, culminado: null, certificado: '', url_certificado: '', instructor: 'Academia de Joystick', description: 'Aprende a crear un sitio corporativo desde cero utilizando sass, css3, jQuery y herramientas profesionales de desarrollo.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'sass','css','html5','jquery' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="99" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -23332,7 +23344,7 @@
         <v>{ id: 98, name: 'LESS de 0 a 100', category: 'Preprocesadores de css', technology: 'Less', url: 'https://www.youtube.com/playlist?list=PLCTD_CpMeEKT70itw70uVs0vlFbvbCPQN', platform: 'YouTube', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 80, culminado: null, certificado: '', url_certificado: '', instructor: 'Programador Novato', description: 'En este tutorial vamos a prender a instalar Less en nuestros proyectos web.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'youtube', logo_technologies: [ 'less' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="100" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
         <v>99</v>
       </c>
@@ -23496,7 +23508,7 @@
         <v>{ id: 99, name: 'javascript Full- Curso desde Principiante hasta Profesional', category: 'Front-end', technology: 'javascript', url: 'https://www.udemy.com/course/javascript-moderno-para-principiantes', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 940, culminado: null, certificado: '', url_certificado: '', instructor: 'Grover Vásquez', description: 'javascript Moderno para principiantes, aprende Fundamentos, POO, ES6+, ajax, WebPack, firebase y Ejemplos de aplicación.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'javascript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="101" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A101" s="5">
         <v>100</v>
       </c>
@@ -23659,7 +23671,7 @@
         <v>{ id: 100, name: 'WEBPACK 5 - ¡Curso práctico DESDE CERO! ', category: 'Empaquetador de javascript', technology: 'Webpack', url: 'https://www.youtube.com/watch?v=FMNuTj89RzU', platform: 'YouTube', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 45, culminado: null, certificado: '', url_certificado: '', instructor: 'Midudev', description: 'Aprende a utilizar WEBPACK 5, el empaquetador de aplicaciones web más utilizado del momento. Veremos cómo crear paso a paso una aplicación con React, cómo crear nuestro entorno de desarrollo y optimizarla.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'youtube', logo_technologies: [ 'webpack' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="102" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A102" s="6">
         <v>101</v>
       </c>
@@ -23832,7 +23844,7 @@
         <v>{ id: 101, name: 'Fundamentos de Marketing Digital', category: 'Soportes', technology: 'Marketing', url: 'https://learndigital.withgoogle.com/activate/course/digital-marketing', platform: 'Google Activate', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 2400, culminado: '2020-05-30', certificado: 'BCU 7HW MSA', url_certificado: 'https://learndigital.withgoogle.com/activate/validate-certificate-code', instructor: 'Google EMEA', description: 'Aprende los conceptos básicos del marketing digital e impulsa tu negocio o tu carrera.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'google', logo_technologies: [ 'generico' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="103" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A103" s="6">
         <v>102</v>
       </c>
@@ -24002,7 +24014,7 @@
         <v>{ id: 102, name: 'Curador de datos', category: 'Bases de datos', technology: 'General', url: 'https://capacitateparaelempleo.org/pages.php?r=.tema&amp;tagID=936', platform: 'Fundación Carlos Slim', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 1440, culminado: '2020-05-31', certificado: '', url_certificado: 'https://capacitateparaelempleo.org/verifica/neglddar1', instructor: 'Capacítate para el empleo', description: 'Aprende a a administrar, crear, manejar y optimizar una base de datos, mediante un software especializado, para que la información sea útil y se convierta en un activo importante para la toma de decisiones.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: false, logo_platform: 'cpee', logo_technologies: [ 'mariadb','heidisql','sql' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="104" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A104" s="6">
         <v>103</v>
       </c>
@@ -24175,7 +24187,7 @@
         <v>{ id: 103, name: 'Curso de Desarrollo de Apps Móviles', category: 'Soportes', technology: 'Desarrollo móvil', url: 'https://learndigital.withgoogle.com/activate/course/apps', platform: 'Google Activate', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 2400, culminado: '2020-06-01', certificado: 'FDH 3RR UEQ', url_certificado: 'https://learndigital.withgoogle.com/activate/validate-certificate-code', instructor: 'Google EMEA', description: 'Descubre el mundo de la Desarrollo de Apps Móviles de la mano de la UCM (Universidad Complutense de Madrid).', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'google', logo_technologies: [ 'androidstudio','xcode','html5','css','javascript','apachecordova' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="105" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A105" s="6">
         <v>104</v>
       </c>
@@ -24348,7 +24360,7 @@
         <v>{ id: 104, name: 'Transformación digital para el empleo', category: 'Soportes', technology: 'General', url: 'https://learndigital.withgoogle.com/activate/course/digital-transformation', platform: 'Google Activate', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 2400, culminado: '2020-06-11', certificado: 'RB5 QF8 D3F', url_certificado: 'https://learndigital.withgoogle.com/activate/validate-certificate-code', instructor: 'Google EMEA', description: 'Descubre todo lo relacionado con la transformación digital de la mano de EOI (Escuela de Organización Industrial).', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'google', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="106" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A106" s="6">
         <v>105</v>
       </c>
@@ -24518,7 +24530,7 @@
         <v>{ id: 105, name: 'Programador (orientado a objetos)', category: 'Paradigmas', technology: 'POO', url: 'https://capacitateparaelempleo.org/pages.php?r=.tema&amp;tagID=4244&amp;load=4255&amp;n=0&amp;brandID=capacitate', platform: 'Fundación Carlos Slim', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 1920, culminado: '2020-06-17', certificado: '', url_certificado: 'https://capacitateparaelempleo.org/verifica/2zg904spc/', instructor: 'Capacítate para el empleo', description: 'Conocerás los conceptos que definen que es la programación y para que sirve.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: false, logo_platform: 'cpee', logo_technologies: [ 'generico' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="107" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A107" s="6">
         <v>106</v>
       </c>
@@ -24688,7 +24700,7 @@
         <v>{ id: 106, name: 'Desarrollador Front-end', category: 'Front-end', technology: 'General', url: 'https://capacitateparaelempleo.org/pages.php?r=.tema&amp;tagID=6726', platform: 'Fundación Carlos Slim', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 1920, culminado: '2020-06-22', certificado: '', url_certificado: 'https://capacitateparaelempleo.org/verifica/undrjn3bg/', instructor: 'Capacítate para el empleo', description: 'Utiliza las tecnologías de la información y comunicación para plasmar el contenido de manera que los usuarios lo puedan aprovechar al máximo.', url_aux: '', calificacion: 'Bueno', actualizado: false, en_ruta: false, logo_platform: 'cpee', logo_technologies: [ 'html5','css','javascript' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="108" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A108" s="6">
         <v>107</v>
       </c>
@@ -24861,7 +24873,7 @@
         <v>{ id: 107, name: 'Competencias digitales para profesionales', category: 'Soportes', technology: 'General', url: 'https://learndigital.withgoogle.com/activate/course/digital-skills', platform: 'Google Activate', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 2400, culminado: '2020-06-25', certificado: 'LLW 86Q BUZ', url_certificado: 'https://learndigital.withgoogle.com/activate/validate-certificate-code', instructor: 'Álvaro Retorillo Osuna', description: 'Descubre la importancia de las competencias digitales para los profesionales de la mano de la Fundación Santa María la Real.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'google', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="109" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A109" s="5">
         <v>108</v>
       </c>
@@ -25025,7 +25037,7 @@
         <v>{ id: 108, name: 'Estructura de Computadores con Arduino Zero', category: 'Soportes', technology: 'General', url: 'https://www.udemy.com/course/estructura-de-computadores-con-arduino-zero', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 98, culminado: null, certificado: '', url_certificado: '', instructor: 'María José Santofimia Romero', description: 'Explorando la estructura básica de un computador.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="110" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A110" s="7">
         <v>109</v>
       </c>
@@ -25189,7 +25201,7 @@
         <v>{ id: 109, name: 'Vue js 3 [Actualizado] ¡De 0 a Experto! + firebase + MEVN', category: 'Frameworks de JavaScript', technology: 'Vue JS', url: 'https://www.udemy.com/course/curso-vue', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 1, minutos: 2396, culminado: null, certificado: '', url_certificado: '', instructor: 'Ignacio Gutiérrez ', description: 'Vue.js 2 y Vue.js 3! Aprende desde 0, Composition API, Vuex, Rutas protegidas, Vue CLI, Nuxt.js, Node, express y mongodb.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'mongo','express','vuejs','nodejs','firebase' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="111" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A111" s="10">
         <v>110</v>
       </c>
@@ -25353,7 +25365,7 @@
         <v>{ id: 110, name: 'Guía completa de GraphQL con angular de 0 a Experto', category: 'Paradigmas', technology: 'GraphQL', url: 'https://www.udemy.com/course/graphql-angular-de-0-a-experto-jwt-socket-mongodb-heroku-anartz-mugika', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: false, priority: 0, minutos: 640, culminado: null, certificado: '', url_certificado: '', instructor: 'Anartz Mugika Ledo', description: 'APIs en Apollo Server express 2 / 3, Testing, Apollo Client, JWT, Apps en tiempo real, mongodb, Hasura, Deploy.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'graphql','angular' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="112" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A112" s="7">
         <v>111</v>
       </c>
@@ -25690,7 +25702,7 @@
         <v>{ id: 112, name: 'Laravel y OAuth 2: Login con Facebook, Twitter, Google+, etc', category: 'Frameworks de back-end', technology: 'Laravel', url: 'https://www.udemy.com/course/laravel-y-oauth-2-facebook-twitter-google', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 0, minutos: 407, culminado: '2022-02-25', certificado: 'UC-035a82e5-ca87-43b3-bf11-a2ee4b3b2705', url_certificado: 'https://www.udemy.com/certificate/UC-035a82e5-ca87-43b3-bf11-a2ee4b3b2705', instructor: 'Juan Ramos', description: 'Desarrollemos un monitor de precios! Los usuarios ingresan vía redes sociales, ingresan datos y consultan reportes.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'laravel','oauth2','facebook','google','twitter','excel' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="114" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A114" s="6">
         <v>113</v>
       </c>
@@ -25866,7 +25878,7 @@
         <v>{ id: 113, name: 'Aprende a publicar cualquier web en Internet (Hosting y VPS)', category: 'Deploy', technology: 'General', url: 'https://www.udemy.com/course/aprende-a-publicar-sitios-web-en-internet-hosting-vps', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 0, minutos: 349, culminado: '2022-02-09', certificado: 'UC-70a57832-6af5-46bc-a638-b13009c9c869', url_certificado: 'https://www.udemy.com/certificate/UC-70a57832-6af5-46bc-a638-b13009c9c869', instructor: 'Víctor Robles', description: 'Sube tus webs creadas con HTML, css, javascript, php, mysql, angular, Node, Mongo, laravel, Symfony, WP, python y django', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'devops','mysql','mongo','laravel','angular','nodejs' ], mostrar: true, repositorio: 'https://github.com/petrix12/deploy_2022.git', nota: '' },</v>
       </c>
     </row>
-    <row r="115" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A115" s="6">
         <v>114</v>
       </c>
@@ -26039,7 +26051,7 @@
         <v>{ id: 114, name: 'Curso Profesional de JAVA', category: 'Lenguajes de Programación', technology: 'Java', url: 'https://codigofacilito.com/cursos/java-profesional', platform: 'Códigofacilito', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 362, culminado: '2020-06-27', certificado: ' 48a2c72e-ba9e-4f7c-ad76-6631dbacf761', url_certificado: 'https://codigofacilito.com/user_quizzes/94372.pdf', instructor: 'Eduardo Ismael García Pérez', description: 'Curso Profesional de JAVA', url_aux: '', calificacion: 'Bueno', actualizado: false, en_ruta: false, logo_platform: 'codigofacilito', logo_technologies: [ 'java' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="116" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A116" s="6">
         <v>115</v>
       </c>
@@ -26209,7 +26221,7 @@
         <v>{ id: 115, name: 'Desarrollador Back-end', category: 'Back-end', technology: 'General', url: 'https://capacitateparaelempleo.org/pages.php?r=.tema&amp;tagID=6725', platform: 'Fundación Carlos Slim', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 1920, culminado: '2020-06-30', certificado: '', url_certificado: 'https://capacitateparaelempleo.org/verifica/o0skcnx58', instructor: 'Capacítate para el empleo', description: 'Utiliza lenguajes de programación para desarrollar módulos de procesamiento que otorguen a los usuarios contenido dinámico basado en las petriciones de entrada. Almacena información de valor utilizando bases de datos y otorga un alto nivel operacional a sitios como las redes sociales, páginas de compras por internet y a la mayoría de páginas web actuales.', url_aux: '', calificacion: 'Regular', actualizado: false, en_ruta: false, logo_platform: 'cpee', logo_technologies: [ 'generico' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="117" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A117" s="6">
         <v>116</v>
       </c>
@@ -26382,7 +26394,7 @@
         <v>{ id: 116, name: 'Programación Básica', category: 'Front-end', technology: 'javascript', url: 'https://platzi.com/clases/1050-programacion-basica/5104-que-es-htmlcssjs', platform: 'Platzi', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 2400, culminado: '2020-07-03', certificado: '10dceb04-40a2-4d14-bb70-ac91648472f6', url_certificado: 'https://platzi.com/@pedro-bazo', instructor: 'John Freddy Vega', description: 'Programación básica con javascript.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: true, logo_platform: 'platzi', logo_technologies: [ 'javascript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="118" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A118" s="6">
         <v>117</v>
       </c>
@@ -26555,7 +26567,7 @@
         <v>{ id: 117, name: 'Curso de introducción a la programación', category: 'Paradigmas', technology: 'General', url: 'https://codigofacilito.com/cursos/introduccion', platform: 'Códigofacilito', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 76, culminado: '2020-07-06', certificado: '7694d69c-ace0-4135-a7ad-d7666cb89493', url_certificado: 'https://codigofacilito.com/user_quizzes/95588.pdf', instructor: 'Petriz Celaya', description: 'Aprende los fundamentos y bases de la programación. Descubre cómo es que con instrucciones de código puedes indicarle a una computadora cómo completar una tarea.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'codigofacilito', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="119" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A119" s="6">
         <v>118</v>
       </c>
@@ -26728,7 +26740,7 @@
         <v>{ id: 118, name: 'Curso de Marca Personal', category: 'Paradigmas', technology: 'General', url: 'https://platzi.com/cursos/marca-personal', platform: 'Platzi', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 720, culminado: '2020-07-06', certificado: '5d15e657-ae42-405c-94de-bbc3ebc7f6e7', url_certificado: 'https://platzi.com/@pedro-bazo', instructor: 'John Freddy Vega', description: 'Construir un portafolio de proyectos y fortalecer tu presencia online te ayudará a resaltar para ampliar tus oportunidades laborales, conseguir un mejor empleo o crear tu propio negocio.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'platzi', logo_technologies: [ 'facebook','instagram','twitter','google','whatsapp' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="120" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A120" s="6">
         <v>119</v>
       </c>
@@ -26901,7 +26913,7 @@
         <v>{ id: 119, name: 'Cloud Computing', category: 'Cloud Computing', technology: 'General', url: 'https://learndigital.withgoogle.com/activate/course/cloud-computing', platform: 'Google Activate', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 2400, culminado: '2020-07-11', certificado: 'BMC RVW BN7', url_certificado: 'https://learndigital.withgoogle.com/activate/validate-certificate-code', instructor: 'Google EMEA', description: 'Descubre el mundo del Cloud Computing de la mano de EOI (Escuela de Organización Industrial)', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'google', logo_technologies: [ 'aws','google','azure','digitalocean' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="121" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A121" s="6">
         <v>120</v>
       </c>
@@ -27073,7 +27085,7 @@
         <v>{ id: 120, name: 'Fundamentos del desarrollo web: Full Stack o Front-end', category: 'Stack', technology: 'General', url: 'https://es.linkedin.com/learning/fundamentos-del-desarrollo-web-full-stack-o-front-end/presentacion-del-curso-fundamentos-del-desarrollo-web-full-stack-o-front-end', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 55, culminado: '2020-07-12', certificado: 'AQoG5v-if5GvR4ih5nmi33igT7HQ', url_certificado: 'https://www.linkedin.com/learning/certificates/f615bb94f4833b31f3b997ff6036441bd36e1fd011d70911b25d934c942a1aab?trk=share_certificate', instructor: 'Sergio Brito', description: 'En este curso aprenderás todo lo que implica ser un desarrollador web, desde las herramientas y frameworks de trabajo necesarias hasta todo lo que debes de considerar para hacerte de un buen trabajo. Descubre qué habilidades deberás poseer y mejorar para ser un profesional exitoso en la industria web.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'linkedin', logo_technologies: [ 'generico' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="122" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A122" s="6">
         <v>121</v>
       </c>
@@ -27243,7 +27255,7 @@
         <v>{ id: 121, name: 'Aprende Visual Studio Code', category: 'Herramientas', technology: 'VS Code', url: 'https://www.linkedin.com/learning/aprende-visual-studio-code', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 85, culminado: '2020-07-13', certificado: 'AdJbdvjorzaWEPQKsR_ruv28nelk', url_certificado: '', instructor: 'Sergio Brito', description: 'Aprende a utilizar Visual Studio Code.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'linkedin', logo_technologies: [ 'vsc' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="123" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A123" s="6">
         <v>122</v>
       </c>
@@ -27416,7 +27428,7 @@
         <v>{ id: 122, name: 'javascript esencial', category: 'Front-end', technology: 'javascript', url: 'https://www.linkedin.com/learning/javascript-esencial/presentacion-del-curso-javascript-esencial', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 327, culminado: '2020-07-15', certificado: 'AfnYV01thUHoafVxBRr5i7RUkTgk', url_certificado: 'https://www.linkedin.com/learning/certificates/6c6262935ed9c6ab5fcac15726fe8fed685f66a160b2fbd04719f8c8abf41487?trk=share_certificate', instructor: 'Sergio Brito', description: 'Conoce javascript, sus clases y elementos, desde sus conceptos más básicos hasta las herramientas más avanzadas. Este curso esencial de javascript, el lenguaje que rige la web, considera la nueva especificación del lenguaje ES6 y te enseña desde los fundamentos hasta un nivel intermedio, de un lenguaje utilizado en distintas áreas, como web, aplicaciones móviles y aplicaciones escritorio. Esto hace de javascript uno de los lenguajes más estudiados y demandados.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'linkedin', logo_technologies: [ 'javascript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="124" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A124" s="6">
         <v>123</v>
       </c>
@@ -27589,7 +27601,7 @@
         <v>{ id: 123, name: 'javascript avanzado: Buenas prácticas', category: 'Front-end', technology: 'javascript', url: 'https://www.linkedin.com/learning/javascript-avanzado-buenas-practicas/presentacion-del-curso-javascript-avanzado-buenas-practicas', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 109, culminado: '2020-07-17', certificado: 'AbEiI_V1GjZq7_M4bBkvg0kwMGwc', url_certificado: 'https://www.linkedin.com/learning/certificates/66a8440ec2362e38b6b8e729e5b131c47a0608b0e7f50cce5c591cbd5b1475ff?trk=share_certificate', instructor: 'Sergio Brito', description: 'En este curso conocerás las buenas prácticas más populares y eficaces, que harán que tu trabajo como desarrollador usando javascript mejore y sea más práctico al trabajar en una nueva aplicación web. Estas buenas prácticas se convertirán en el set de acciones que incorporarás en cada proyecto web y que ayudarán a que tu código sea mejor.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'linkedin', logo_technologies: [ 'javascript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="125" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A125" s="6">
         <v>124</v>
       </c>
@@ -27762,7 +27774,7 @@
         <v>{ id: 124, name: 'javascript avanzado: Expresiones regulares', category: 'Front-end', technology: 'javascript', url: 'https://www.linkedin.com/learning/javascript-avanzado-expresiones-regulares/presentacion-del-curso-javascript-avanzado-expresiones-regulares', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 94, culminado: '2020-07-18', certificado: 'AcULzI6GeFyOA5dRitATMcLFJ2ik', url_certificado: 'https://www.linkedin.com/learning/certificates/d7f64256de10f5ab340fa733d2760aface893e774bad1551394104533bcadc78?trk=share_certificate', instructor: 'Sergio Brito', description: 'Aprende en este curso a usar las expresiones regulares con javascript.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'linkedin', logo_technologies: [ 'javascript' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="126" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A126" s="6">
         <v>125</v>
       </c>
@@ -27932,7 +27944,7 @@
         <v>{ id: 125, name: 'Node.js esencial', category: 'Back-end', technology: 'Node.js', url: 'https://www.linkedin.com/learning/node-js-esencial', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 222, culminado: '2020-07-20', certificado: 'AXBaLkGLNI7CeQhU2t3l4DJDAkcH', url_certificado: '', instructor: 'Carlos Solís', description: 'En este curso, vamos a explorar todo lo que necesitas saber para comenzar a trabajar ya con Node.js. Veremos los pasos básicos de instalación, las reglas básicas de sintaxis y cómo crear aplicaciones completas. Después de este curso, podrás dar los primeros pasos para convertirte en un desarrollador Fullstack.', url_aux: '', calificacion: 'Muy bueno', actualizado: false, en_ruta: false, logo_platform: 'linkedin', logo_technologies: [ 'nodejs' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="127" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A127" s="6">
         <v>126</v>
       </c>
@@ -28102,7 +28114,7 @@
         <v>{ id: 126, name: 'Node.js práctico: Sitio web', category: 'Back-end', technology: 'Node.js', url: 'https://www.linkedin.com/learning/node-js-practico-sitio-web', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 82, culminado: '2020-07-24', certificado: 'AUlU2edpTPRe9X3Vt9JzJ5eo8z7N', url_certificado: '', instructor: 'Carlos Solís', description: 'En este curso práctico nos enfocaremos en diferentes proyectos web basados en nodejs. Crearemos un sitio completo y utilizaremos funciones avanzadas, así como librerías y servicios adicionales para llevar nuestro producto al siguiente nivel. Finalmente aprenderemos los procesos de publicación en diferentes servicios en la nube para que nuestra aplicación esté disponible para el mundo entero.', url_aux: '', calificacion: 'Muy bueno', actualizado: false, en_ruta: false, logo_platform: 'linkedin', logo_technologies: [ 'nodejs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="128" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A128" s="6">
         <v>127</v>
       </c>
@@ -28271,7 +28283,7 @@
         <v>{ id: 127, name: 'Aprende diseño de base de datos relacionales', category: 'Bases de datos', technology: 'General', url: 'https://www.linkedin.com/learning/aprende-diseno-de-base-de-datos-relacionales', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 53, culminado: '2020-07-28', certificado: 'Ae5V_EEcB2xVaK6WTCpW6_QF21d6', url_certificado: '', instructor: 'Noemí León', description: '¿Quieres iniciarte en el mundo de las bases de datos y no sabes por dónde empezar? ¿Tienes un sitio web y quieres agregarle una base de datos, pero no entiendes muchos conceptos? En este curso, partiremos de los conceptos básicos. Veremos qué es una base de datos y cuáles son sus clasificaciones principales, hasta llegar a conceptos precisos del diseño de bases de datos relacionales, de forma que, cuando termines el curso, tendrás una idea clara de cómo funcionan este tipo de bases de datos y si están hechas para ti.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'linkedin', logo_technologies: [ 'sql' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="129" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A129" s="6">
         <v>128</v>
       </c>
@@ -30806,7 +30818,7 @@
         <v>{ id: 142, name: 'Desplegar tu proyecto laravel en Digital Ocean', category: 'Deploy', technology: 'Laravel', url: 'https://www.youtube.com/playlist?list=PLZ2ovOgdI-kWRdVAJLH0kEHSNKCk8rz_x', platform: 'YouTube', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 90, culminado: '2021-03-19', certificado: 'S/C', url_certificado: '', instructor: 'Victor Arana Flores', description: 'En esta nueva serie te enseñaré a cómo administrar tu propio servidor, y subir tus proyectos laravel en él.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'youtube', logo_technologies: [ 'laravel','digitalocean' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="144" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A144" s="6">
         <v>143</v>
       </c>
@@ -30976,7 +30988,7 @@
         <v>{ id: 143, name: 'Vue.js desde cero', category: 'Frameworks de JavaScript', technology: 'Vue JS', url: 'https://aprendible.com/series/vuejs-desde-cero', platform: 'Aprendible', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 70, culminado: '2021-04-28', certificado: 'S/C', url_certificado: '', instructor: 'Jorge Luis García Coello', description: 'En esta serie aprenderemos a utilizar Vue.js desde cero y cómo integrarlo en tus aplicaciones de laravel.', url_aux: '', calificacion: 'Muy bueno', actualizado: false, en_ruta: false, logo_platform: 'aprendible', logo_technologies: [ 'vuejs' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="145" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A145" s="6">
         <v>144</v>
       </c>
@@ -31315,7 +31327,7 @@
         <v>{ id: 145, name: 'Relaciones avanzadas de laravel', category: 'Frameworks de back-end', technology: 'Laravel', url: 'https://codersfree.com/cursos/relaciones-avanzadas-de-laravel', platform: 'Coders Free', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 180, culminado: '2021-07-29', certificado: 'S/C', url_certificado: '', instructor: 'Victor Arana Flores', description: 'En este curso aprenderás a como trabajar con una base de datos en un proyecto real.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'coders_free', logo_technologies: [ 'laravel' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="147" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A147" s="6">
         <v>146</v>
       </c>
@@ -31484,7 +31496,7 @@
         <v>{ id: 146, name: 'Programación Orientada a Objetos y principios SOLID', category: 'Paradigmas', technology: 'POO', url: 'https://www.udemy.com/course/programacion-orientada-a-objetos-y-principio-solid', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 51, culminado: '2021-08-27', certificado: 'S/C', url_certificado: '', instructor: 'Eduardo Patiño', description: 'Curso conceptual sobre el paradigma de la programación orientada a objetos y SOLID.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="148" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A148" s="6">
         <v>147</v>
       </c>
@@ -31654,7 +31666,7 @@
         <v>{ id: 147, name: 'Las bases para desarrollar una aplicación full stack MERN', category: 'Stack', technology: 'MERN', url: 'https://www.udemy.com/course/las-bases-para-desarrollar-una-aplicacion-full-stack-mern', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 74, culminado: '2021-11-20', certificado: 'S/C', url_certificado: '', instructor: 'Luis Trujillo Sánchez', description: 'Aprende las bases para crear una aplicación web con el stack MERN (mongodb, express, react, nodejs)', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'mongo','express','reactjs','nodejs' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="149" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A149" s="6">
         <v>148</v>
       </c>
@@ -32000,7 +32012,7 @@
         <v>{ id: 149, name: 'Aprende a crear una plataforma de cursos con laravel', category: 'Frameworks de back-end', technology: 'Laravel', url: 'https://codersfree.com/cursos/aprende-a-crear-una-plataforma-de-cursos-con-laravel', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 0, minutos: 1320, culminado: '2021-06-21', certificado: 'UC-808bf328-9ed5-4792-bcd3-755dde0f62f6', url_certificado: 'https://www.udemy.com/certificate/UC-808bf328-9ed5-4792-bcd3-755dde0f62f6', instructor: 'Victor Arana Flores', description: 'En este curso aprenderás a crear una plataforma de cursos, con laravel, Livewire Tailwind y Alpine.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'laravel','livewire','tailwindcss','alpine' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="151" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A151" s="6">
         <v>150</v>
       </c>
@@ -32173,7 +32185,7 @@
         <v>{ id: 150, name: 'Desarrollo web : HTML, css, javascript, JQuery, python y django', category: 'Stack', technology: 'python-django', url: 'https://www.udemy.com/course/desarrollo-web-con-python-y-django', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 649, culminado: '2021-07-02', certificado: 'UC-f64e78a2-26a3-4ef5-84e8-0b22058eb52a', url_certificado: 'https://www.udemy.com/certificate/UC-f64e78a2-26a3-4ef5-84e8-0b22058eb52a', instructor: 'Redait Media', description: 'Aprende a construir sitios web con HTML, css, bootstrap, javascript, JQuery, python 3 y django.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'html5','css','javascript','jquery','python','django' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="152" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A152" s="6">
         <v>151</v>
       </c>
@@ -32346,7 +32358,7 @@
         <v>{ id: 151, name: 'Aprende a instalar laravel 8 en Amazon Web Services', category: 'Deploy', technology: 'AWS', url: 'https://www.udemy.com/course/draft/3793886/learn/lecture/24522234?start=0#overview', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 0, minutos: 90, culminado: '2021-07-29', certificado: 'UC-a7113805-8cb5-405b-9791-5c134e6d8e3c', url_certificado: 'https://www.udemy.com/certificate/UC-a7113805-8cb5-405b-9791-5c134e6d8e3c', instructor: 'Homero Raúl Vargas Cruz', description: 'Instalación de laravel en Amazon EC2, configuracion de la base de datos, implementar certificado SSL y mucho más.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'aws','laravel' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="153" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A153" s="6">
         <v>152</v>
       </c>
@@ -32519,7 +32531,7 @@
         <v>{ id: 152, name: 'La ruta del desarrollador web', category: 'Paradigmas', technology: 'General', url: 'https://app.ed.team/cursos/web', platform: 'EDteam', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 180, culminado: '2021-07-30', certificado: '228409405-1cd51139-1307-460e-abc8-d6890e6b85bc', url_certificado: 'https://app.ed.team/@pedrojesusbazocanelon/curso/web', instructor: 'Alvaro Felipe Chávez', description: 'Aprende todos los roles y rutas que existen para ser un desarrollador web profesional en 2021.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'edteam', logo_technologies: [ 'generico' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="154" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A154" s="6">
         <v>153</v>
       </c>
@@ -32691,7 +32703,7 @@
         <v>{ id: 153, name: 'Introducción a API REST', category: 'Paradigmas', technology: 'API RESTful', url: 'https://app.ed.team/cursos/api-rest', platform: 'EDteam', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 60, culminado: '2021-07-30', certificado: '228409382-1a5a5de0-fcf7-4f3f-95f4-531b23188ba3', url_certificado: 'https://app.ed.team/@pedrojesusbazocanelon/curso/api-rest', instructor: 'Alexys Lozada', description: 'Aprende todos los conceptos teóricos que hay en la arquitectura REST.', url_aux: '', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'edteam', logo_technologies: [ 'apirestful' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="155" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A155" s="6">
         <v>154</v>
       </c>
@@ -32864,7 +32876,7 @@
         <v>{ id: 154, name: 'Introducción a Google Cloud Platform', category: 'Cloud Computing', technology: 'Google Cloud Platform', url: 'https://www.udemy.com/course/introduccion-a-google-cloud-platform', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 210, culminado: '2021-08-03', certificado: 'UC-8d986592-d2d2-42bd-971b-61f25426f6a1', url_certificado: 'https://www.udemy.com/certificate/UC-8d986592-d2d2-42bd-971b-61f25426f6a1', instructor: 'Josue Guevara', description: 'Aprende los fundamentos de los servicios de GCP y desarolla miniproyectos dentro de la plataforma de Google', url_aux: '', calificacion: 'Regular', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'google' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="156" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A156" s="6">
         <v>155</v>
       </c>
@@ -33040,7 +33052,7 @@
         <v>{ id: 155, name: 'Graba y transmite cursos online', category: 'Herramientas', technology: 'OBS Studio', url: 'https://app.ed.team/cursos/curso-online', platform: 'EDteam', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 240, culminado: '2021-08-07', certificado: '228409385-ce9e27be-d058-4ab8-a6ef-3a465eb73ffc', url_certificado: 'https://app.ed.team/u/pedrojesusbazocanelon/curso/curso-online', instructor: 'Alvaro Felipe Chávez', description: 'Aprende a crear cursos para YouTube, EDteam, Twitch u otras plataformas de la mano de nuestros expertos.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'edteam', logo_technologies: [ 'obs' ], mostrar: false, repositorio: 'https://github.com/petrix12/obs-grabar-cursos-2021', nota: '' },</v>
       </c>
     </row>
-    <row r="157" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A157" s="6">
         <v>156</v>
       </c>
@@ -33389,7 +33401,7 @@
         <v>{ id: 157, name: 'Crea una pasarela de pagos con laravel Cashier y Stripe', category: 'Frameworks de back-end', technology: 'Laravel', url: 'https://codersfree.com/cursos/crea-una-pasarela-de-pagos-con-laravel', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 0, minutos: 300, culminado: '2021-09-23', certificado: 'UC-afccdce2-6ca4-4e43-a222-68a681897c55', url_certificado: 'https://www.udemy.com/certificate/UC-afccdce2-6ca4-4e43-a222-68a681897c55', instructor: 'Victor Arana Flores', description: 'En este curso aprenderás a implementar una pasarela de pagos completa en tu negocio virtual.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'laravel','stripe' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="159" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A159" s="6">
         <v>158</v>
       </c>
@@ -33562,7 +33574,7 @@
         <v>{ id: 158, name: 'CRUD con php mysql bootstrap jQuery ajax y Docker', category: 'Herramientas', technology: 'Docker', url: 'https://www.udemy.com/course/crud-con-php-mysql-bootstrap-jquery-ajax-y-docker', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 90, culminado: '2021-12-13', certificado: 'UC-266882f9-ff9e-40f2-8218-45945c338c1b', url_certificado: 'https://www.udemy.com/certificate/UC-266882f9-ff9e-40f2-8218-45945c338c1b', instructor: 'Wener Ovalle', description: 'Aprende hacer una aplicación web por medio de un proyecto práctico con tu entorno de desarrollo hecho en Docker.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'php','mysql','bootstrap','jquery','ajax','docker' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="160" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A160" s="6">
         <v>159</v>
       </c>
@@ -33735,7 +33747,7 @@
         <v>{ id: 159, name: 'Web Personal MERN Full Stack: mongodb, express, React y Node', category: 'Stack', technology: 'MERN', url: 'https://www.udemy.com/course/web-personal-mern-full-stack-mongodb-express-react-node', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 0, minutos: 2010, culminado: '2021-12-22', certificado: 'UC-c5c360e3-a8c2-4ed7-a285-64e4b7c28a02', url_certificado: 'https://www.udemy.com/certificate/UC-c5c360e3-a8c2-4ed7-a285-64e4b7c28a02', instructor: 'Agustin Navarro Galdón', description: 'Desarrollo Full Stack, creando una web personal con el Stack MERN (mongodb, express, React y Node) la ultima tecnología.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'mongo','express','reactjs','nodejs' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="161" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A161" s="6">
         <v>160</v>
       </c>
@@ -33908,7 +33920,7 @@
         <v>{ id: 160, name: 'Aprende big data: Análisis de datos', category: 'Big Data', technology: 'General', url: 'https://www.linkedin.com/learning/aprende-big-data-analisis-de-datos/que-es-el-big-data-2', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 110, culminado: '2020-09-25', certificado: 'AYRhj01XBJa1w32_eXe-0-dKz09M', url_certificado: 'https://www.linkedin.com/learning/certificates/6d1d9c5613b30cf9052cde2b84cb3a99cf2c2784af8bb49ffc54407b527a3f0b?trk=share_certificate', instructor: 'Ana María Bisbé York', description: 'Aprende big data para la empresa de hoy, desde las bases fundamentales a los roles más específicos de la ciencia de los datos. Conoce a qué nos referimos con big data y por qué es necesario estar al día en esta tecnología para sobrevivir en el ecosistema empresarial. Expande tus conocimientos sobre la presencia del big data en nuestras vidas y en las tecnologías que la rodean, y entiende cómo sacar mayor partido a este futuro reciente en tu propia empresa.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'linkedin', logo_technologies: [ 'generico' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="162" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A162" s="6">
         <v>161</v>
       </c>
@@ -34081,7 +34093,7 @@
         <v>{ id: 161, name: 'Big data: Escucha activa', category: 'Big Data', technology: 'General', url: 'https://www.linkedin.com/learning/big-data-escucha-activa/presentacion-del-curso-big-data-escucha-activa', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 89, culminado: '2020-09-15', certificado: 'AZa4uEbUurHG4V_TUoX9xcrUXr6R', url_certificado: 'https://www.linkedin.com/learning/certificates/51b6604bebb327dd7bc6f86eca2acca16ec0fd62c9e7191db5de3b01e6a86ffb?trk=share_certificate', instructor: 'Míriam Hatibi Zagmal', description: 'Escuchar lo que tus clientes o el mercado opinan de tu producto, servicio o empresa es parte de la estrategia que toda empresa debe tener en pie. Las redes sociales son extremadamente útiles para este fin. Con este curso, entenderás qué es la escucha activa en redes sociales y qué puede ofrecernos. Además, a través de ejemplos prácticos, aprenderás a poner en marcha una estrategia de escucha activa, de principio a fin.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'linkedin', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="163" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A163" s="6">
         <v>162</v>
       </c>
@@ -34250,7 +34262,7 @@
         <v>{ id: 162, name: 'Devops con un café', category: 'Deploy', technology: 'General', url: 'https://www.linkedin.com/learning/devops-con-un-cafe/historia-de-devops', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 10, culminado: '2020-09-08', certificado: '', url_certificado: 'http://www.linkedin.com/learning/devops-con-un-café', instructor: 'Álvaro González Crespo', description: 'Entiende qué es y cómo funciona devops, un acrónimo inglés de "development" (desarrollo) y "operations" (operaciones). Conoce en solo cuatro vídeos esta metodología de desarrollo de software que se centra en la comunicación, colaboración e integración entre los desarrolladores de software y los profesionales de sistemas de tecnologías de la información.', url_aux: '', calificacion: 'Bueno', actualizado: false, en_ruta: false, logo_platform: 'linkedin', logo_technologies: [ 'devops' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="164" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A164" s="6">
         <v>163</v>
       </c>
@@ -34419,7 +34431,7 @@
         <v>{ id: 163, name: 'Cómo hackear tu mente y recuperar el control sobre el estrés', category: 'Otros', technology: 'Otros', url: 'https://www.linkedin.com/learning/como-hackear-tu-mente-y-recuperar-el-control-sobre-el-estres/para-aumentar-tu-productividad-tienes-que-hacer-menos-cosas', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 51, culminado: '2020-09-08', certificado: '', url_certificado: 'http://www.linkedin.com/learning/como-hackear-tu-mente-y-recuperar-el-control-sobre-el-estrés', instructor: 'Izanami Martínez', description: 'Supera el estrés y consigue dejar atrás la sensación de que no tienes tiempo. Aprende qué es, qué le pasa a tu cuerpo cuando se activa o se vuelve crónico, y qué hábitos mentales y nutricionales lo empeoran. Consigue, con este curso, resetear tu mente y recuperar el control de tu día a día con sesiones prácticas de respiración consciente y mindfulness que te devolverán tu claridad mental y tu equilibrio.', url_aux: '', calificacion: 'Bueno', actualizado: false, en_ruta: false, logo_platform: 'linkedin', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="165" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A165" s="6">
         <v>164</v>
       </c>
@@ -34592,7 +34604,7 @@
         <v>{ id: 164, name: 'Fundamentos de big data', category: 'Big Data', technology: 'General', url: 'https://www.linkedin.com/learning/fundamentos-de-big-data/presentacion-del-curso-fundamentos-de-big-data', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 95, culminado: '2020-09-06', certificado: 'AToJuOfwEMn2On9Bc2F5T8eS4ud-', url_certificado: 'https://www.linkedin.com/learning/certificates/b2fa1c97404af07ba2e4d15a8acae90ee97c92e06fb8978ba521d3a561263e10?trk=share_certificate', instructor: 'Míriam Hatibi Zagmal', description: 'Hoy en día, es clave entender las bases del Big Data en nuestro mundo y nuestra realidad. Con este curso, te introducirás en el mundo del Big Data o Macro Datos, y sabrás cómo puede afectarte a ti y a tu empresa. Conocerás la evolución y los avances en Big Data de los últimos años y las diferentes aplicaciones que tiene, para obtener las herramientas necesarias que te permitan aplicarlo a tu organización, independientemente de su sector o tamaño. Conseguirás identificar las mejores formas de optimizar el Big Data adecuándolo a tus recursos o entendiendo qué recursos buscar al externo o desarrollar en tu equipo para poderlo implementar.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'linkedin', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="166" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A166" s="6">
         <v>165</v>
       </c>
@@ -34765,7 +34777,7 @@
         <v>{ id: 165, name: 'Fundamentos de ITIL: Introducción a la gestión de sistemas de información', category: 'IT', technology: 'General', url: 'https://www.linkedin.com/learning/fundamentos-de-itil-introduccion-a-la-gestion-de-sistemas-de-informacion/presentacion-del-curso-fundamentos-de-itil-introduccion-a-la-gestion-de-sistemas-de-informacion', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 84, culminado: '2020-09-03', certificado: 'AW-ExSc3C589ZqRBgJibb5Dvsy9_', url_certificado: 'https://www.linkedin.com/learning/certificates/cf248f02b7ebcb1cf3b7c6aa97792f49ae48a7460c80a1b9a45501bd9f47e6a4?trk=share_certificate', instructor: 'Stéphane Kittler', description: 'La importancia de los sistemas de información en la empresa y el gobierno ya no está en duda. ¿Cómo configurar y cómo administrar un sistema de información de calidad, eficaz en el coste más bajo, a la vez que se cumplen los requerimientos del negocio? ¡ITIL 2011 es la respuesta! Este método es una colección de prácticas de sentido común que pueden adaptarse a cualquier tipo de negocio y sin costo alguno, excepto el tiempo necesario para ponerlo en práctica.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: false, logo_platform: 'linkedin', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="167" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A167" s="6">
         <v>166</v>
       </c>
@@ -34938,7 +34950,7 @@
         <v>{ id: 166, name: 'Fundamentos de la atención al cliente para profesionales IT', category: 'IT', technology: 'General', url: 'https://www.linkedin.com/learning/fundamentos-de-la-atencion-al-cliente-para-profesionales-it/presentacion-del-curso-fundamentos-de-la-atencion-al-cliente-para-profesionales-it', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 73, culminado: '2020-08-31', certificado: ' AflW1bqnkMlJLGcU44m2oka8_VwG', url_certificado: 'https://www.linkedin.com/learning/certificates/7ece58b170fd293c2e72add25e9e8c0117c3a1525407da3b3603c8c6b0398818?trk=share_certificate', instructor: 'Fran Moreno Giménez', description: 'Aprende a construir una relación estable con los clientes de tu negocio de servicios IT. En este curso verás que, en el mundo IT, la atención al cliente y la gestión eficaz de conflictos son parte esencial del negocio. Descubre cómo proporcionar un excepcional servicio al cliente y una buena experiencia que te permita aliviar las frustraciones de manera rápida y profesional, elementos críticos para el éxito a largo plazo de tu empresa de servicios IT.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: false, logo_platform: 'linkedin', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="168" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A168" s="6">
         <v>167</v>
       </c>
@@ -35108,7 +35120,7 @@
         <v>{ id: 167, name: 'SCRUM: Roles', category: 'Metodologías Ágiles', technology: 'SCRUM', url: 'https://www.linkedin.com/learning/scrum-roles', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 101, culminado: '2020-08-25', certificado: '', url_certificado: 'http://www.linkedin.com/learning/scrum-roles', instructor: 'Carlos Solís', description: 'SCRUM es una metodología ágil de gestión de proyectos que se ha convertido prácticamente en el estándar de trabajo de incontables organizaciones y empresas. Es fácil de comprender, y en general no toma mucho tiempo comenzar a aplicarlo en un proyecto. Sin embargo, exige que cada integrante conozca a la perfeccion su rol y el de los demás, para que el proyecto funcione sin fricciones. En este curso, vamos a descubrir las tareas que debe cumplir cada integrante del proyecto y analizaremos cada rol a lo largo del ciclo de vida de un proyecto SCRUM.', url_aux: '', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'linkedin', logo_technologies: [ 'generico' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="169" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A169" s="6">
         <v>168</v>
       </c>
@@ -35284,7 +35296,7 @@
         <v>{ id: 168, name: 'Aprende SCRUM', category: 'Metodologías Ágiles', technology: 'SCRUM', url: 'https://www.linkedin.com/learning/aprende-scrum/presentacion-del-curso-aprende-scrum', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 92, culminado: '2020-08-21', certificado: ' Aa5zDZxQPUZCW-SOb-6dBBPt2Bg5', url_certificado: 'https://www.linkedin.com/learning/certificates/ab2ec26b2e6bc7bdb36eaa9a7f114a4b45c2ca0b6a6fc2124d01b391c660d79b?trk=share_certificate', instructor: 'Carlos Solís', description: 'Descubre SCRUM, la metodología ágil de gestión de proyectos que marca una tendencia en la industria. Desde pequeños startups hasta grandes corporaciones, esta nueva forma de trabajar está revolucionando la forma en que trabajamos en equipo. En este curso aprenderás las bases de la filosofia SCRUM, sus roles, herramientas e implementación. Conocerás los fundamentos principales para comenzar a organizar tus proyectos reduciendo el trabajo innecesario y aumentando sustancialmente la motivación y productividad de tus compañeros de equipo. Aprende qué es y cómo incorporar SCRUM a tus proyectos.', url_aux: 'https://www.linkedin.com/learning/certificates/7c353c20a1a3d6c492bbf7f727f8f8e0130853371c623221cc4440648073f10d?trk=share_certificate', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'linkedin', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="170" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A170" s="6">
         <v>169</v>
       </c>
@@ -35454,7 +35466,7 @@
         <v>{ id: 169, name: 'Fundamentos esenciales de la programación (2014)', category: 'Paradigmas', technology: 'General', url: 'https://www.linkedin.com/learning/fundamentos-esenciales-de-la-programacion-2014', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 348, culminado: '2020-09-02', certificado: '', url_certificado: 'http://www.linkedin.com/learning/fundamentos-esenciales-de-la-programacion', instructor: 'Simon Allardice', description: 'Aprende a desarrollar aplicaciones informáticas en cualquier lenguaje de programación con este curso en el que te explicamos, de la manera más clara y directa posible, cuáles son los componentes comunes a cualquier lenguaje y cuáles son los pasos que tienes que dar para convertir cualquier idea en tu cabeza en una aplicación informática.', url_aux: '', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'linkedin', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="171" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A171" s="6">
         <v>170</v>
       </c>
@@ -35627,7 +35639,7 @@
         <v>{ id: 170, name: 'GitHub para programadores (2016)', category: 'Herramientas', technology: 'GitHub', url: 'https://www.linkedin.com/learning/github-para-programadores-2016/presentacion-del-curso-github-para-programadores-2016', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 113, culminado: '2020-08-06', certificado: 'Ac1TWgJQjZz6PgqkMQvyLVE4vSgx', url_certificado: 'https://www.linkedin.com/learning/certificates/d04eb818dcc9e38983896c5e516fe823f49f18af2fe1a1c2237c66bc17ba59c9?trk=share_certificate', instructor: 'Carlos Solís', description: 'Los equipos de desarrollo modernos necesitan que muchas personas trabajen sobre un mismo código sin generar errores o conflictos. Sin embargo, sin las herramientas adecuadas, esta tarea puede ser casi imposible. Afortunadamente tenemos GitHub, un servicio de control de versiones online que te permite almacenar, gestionar y distribuir tu código. En este curso aprenderás los conceptos básicos del control de versiones Git, los servicios que ofrece GitHub, como crear, gestionar y examinar nuestros repositorios online. Descubrirás diversas formas de utilizar el servicio de GitHub y exploraremos las funciones más comunes de este servicio. Al finalizar este curso estarás a punto para trabajar tu código fuente en equipo con seguridad y la tranquilidad de tener siempre un respaldo en la nube.', url_aux: '', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'linkedin', logo_technologies: [ 'github' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="172" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A172" s="6">
         <v>171</v>
       </c>
@@ -35797,7 +35809,7 @@
         <v>{ id: 171, name: 'Gestión de proyectos simplificada', category: 'Metodologías Ágiles', technology: 'General', url: 'https://www.linkedin.com/learning/gestion-de-proyectos-simplificada', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 86, culminado: '2020-08-16', certificado: '', url_certificado: 'http://www.linkedin.com/learning/gestion-de-proyectos-simplificada', instructor: 'Clara Vega', description: 'Con algunas técnicas sencillas sobre la gestión de proyectos podrás optimizar tu trabajo ya que, en el fondo, casi todo lo que haces en el trabajo es un proyecto; desde la tarea más pequeña hasta tu labor más grande. En este curso, aprenderás los doce pasos de la gestión de proyectos, que podrás aplicar sin mucho esfuerzo, y verás cómo usar herramientas tradicionales de gestión de proyectos, como los diagramas de Gantt y los diagramas de red para que gestiones tu carga de trabajo.', url_aux: '', calificacion: 'Bueno', actualizado: false, en_ruta: false, logo_platform: 'linkedin', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="173" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A173" s="6">
         <v>172</v>
       </c>
@@ -35967,7 +35979,7 @@
         <v>{ id: 172, name: 'Fundamentos de la gestión del tiempo', category: 'Otros', technology: 'Otros', url: 'https://www.linkedin.com/learning/fundamentos-de-la-gestion-del-tiempo', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 88, culminado: '2020-08-13', certificado: '', url_certificado: 'http://www.linkedin.com/learning/fundamentos-de-la-gestion-del-tiempo', instructor: 'Francisco Rábano', description: 'Aprende en este curso a organizarte mejor para disponer de más tiempo de calidad en el que desarrollar tus objetivos y expectativas. Descubre trucos, herramientas, métodos y acciones específicas dirigidas a la mejora de tu eficacia y tu bienestar general, con los que serás capar de tomar mejores decisiones. Mantén más control sobre las tareas a las que dedicas tu tiempo, trabaja tu disciplina, perseverancia y responsabilidad individual, y sustituye el modo reactivo de actuar por el modo reflexivo.', url_aux: '', calificacion: 'Bueno', actualizado: false, en_ruta: false, logo_platform: 'linkedin', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="174" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A174" s="6">
         <v>173</v>
       </c>
@@ -36140,7 +36152,7 @@
         <v>{ id: 173, name: 'Desarrollo web: Control de calidad automatizado', category: 'Paradigmas', technology: 'General', url: 'https://www.linkedin.com/learning/desarrollo-web-control-de-calidad-automatizado/presentacion-del-curso-desarrollo-web-control-de-calidad-automatizado', platform: 'LinkedIn Learning', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 174, culminado: '2020-08-10', certificado: ' AVDow0mkqvN5MsRmSDUrkqkDK7dj', url_certificado: 'https://www.linkedin.com/learning/certificates/6d1d61ea694a83acf3e28722f75e638b723412d06ab9f6499ce7566b1c0bd3d9?trk=share_certificate', instructor: 'Carlos Solís', description: 'Aprende a usar herramientas automatizadas de control de calidad para que tus desarrollos web sean consecuentes y anticiparte a los posibles problemas del código. Automatiza tus pruebas con PhantomJS, CasperJS y Gulp y aprende en este curso a generar informes que te aseguren que cuando un proyecto web sale a producción cumple todos los requisitos.', url_aux: '', calificacion: 'Muy bueno', actualizado: false, en_ruta: false, logo_platform: 'linkedin', logo_technologies: [ 'generico' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="175" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A175" s="6">
         <v>174</v>
       </c>
@@ -36644,7 +36656,7 @@
         <v>{ id: 176, name: 'Crea un Ecommerce con laravel, Livewire, Tailwind y Alpine', category: 'Frameworks de back-end', technology: 'Laravel', url: 'https://codersfree.com/cursos/crea-un-ecommerce-con-laravel-livewire-tailwind-y-alpine', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 1, minutos: 1920, culminado: null, certificado: '', url_certificado: '', instructor: 'Victor Arana Flores', description: 'En este curso aprenderás a desarrollar un ecommerce, con laravel, Livewire, Tailwind y Alpine.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'laravel','livewire','tailwindcss' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="178" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A178" s="6">
         <v>177</v>
       </c>
@@ -36820,7 +36832,7 @@
         <v>{ id: 177, name: 'javascript: Desde cero con nodejs', category: 'Back-end', technology: 'Node.js', url: 'https://www.udemy.com/course/javascript-desde-cero-con-nodejs', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 733, culminado: '2022-10-12', certificado: 'UC-e07a45fb-05c5-4ef2-bb24-25b48d1df14c', url_certificado: 'https://udemy-certificate.s3.amazonaws.com/pdf/UC-e07a45fb-05c5-4ef2-bb24-25b48d1df14c.pdf', instructor: 'Geovanny Gabriel Arguello', description: 'Aprende los fundamentos y crea un proyecto REST API con Node JS.', url_aux: '', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'nodejs','javascript' ], mostrar: false, repositorio: 'https://github.com/petrix12/nodejs2022/tree/main/99-node', nota: '' },</v>
       </c>
     </row>
-    <row r="179" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A179" s="5">
         <v>178</v>
       </c>
@@ -36984,7 +36996,7 @@
         <v>{ id: 178, name: 'Master en python 3.x. Aprende de 0 a EXPERTO con Práctica', category: 'Back-end', technology: 'python', url: 'https://www.udemy.com/course/aprende-el-lenguaje-de-programacion-python3-practicando', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 1530, culminado: null, certificado: '', url_certificado: '', instructor: 'Alvaro Chirou', description: 'Aprende python, donde iniciamos desde 0, sin conocimientos previos hasta desarrollar aplicaciones con mucha practica!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'python' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="180" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A180" s="5">
         <v>179</v>
       </c>
@@ -37148,7 +37160,7 @@
         <v>{ id: 179, name: 'Introducción a la Programación en Varios Lenguajes', category: 'Paradigmas', technology: 'Programación', url: 'https://www.udemy.com/course/programacion-todosloslenguajes', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 115, culminado: null, certificado: '', url_certificado: '', instructor: 'Jorge Salgado Miranda', description: 'python, C, C++, C#, Go, Java, javascript, linux, Swift, Dart, Scala, Kotlin, php, SQL.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="181" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A181" s="5">
         <v>180</v>
       </c>
@@ -37312,7 +37324,7 @@
         <v>{ id: 180, name: 'python y flask. Desarrollo web y APIS tipo REST con flask', category: 'Frameworks de back-end', technology: 'python-flask', url: 'https://www.udemy.com/course/curso-python-y-flask-desarrollo-web-y-apis-tipo-rest', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 639, culminado: null, certificado: '', url_certificado: '', instructor: 'Redait Media', description: 'Aprende HTML, python y flask para el desarrollo de páginas web y la creación de microservicios de tipo REST con flask.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'python','flask' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="182" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A182" s="5">
         <v>181</v>
       </c>
@@ -37476,7 +37488,7 @@
         <v>{ id: 181, name: 'Universidad python con Frameworks django, flask y mucho más!', category: 'Back-end', technology: 'python', url: 'https://www.udemy.com/course/universidad-python-desde-cero-hasta-experto-django-flask-rest-web', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 3692, culminado: null, certificado: '', url_certificado: '', instructor: 'Ubaldo Acosta', description: '+61 hrs De Cero a Experto en python: PySide, Tkinter, Web con django, flask, Jinja, SQL Alchemy, Postgresql y PyCharm!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'python','django','flask' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="183" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A183" s="5">
         <v>182</v>
       </c>
@@ -37640,7 +37652,7 @@
         <v>{ id: 182, name: 'Crea interfaces gráficas para escritorio con python y PyQT', category: 'Lenguajes de Programación', technology: 'python', url: 'https://www.udemy.com/course/crea-interfaces-graficas-para-escritorio-con-python-y-pyqt', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 919, culminado: null, certificado: '', url_certificado: '', instructor: 'Issel Electronics', description: 'Aprende a crear tus propias aplicaciones con la librería más potente para la creación de interfaces graficas con python.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'python','pyqt' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="184" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A184" s="5">
         <v>183</v>
       </c>
@@ -37807,7 +37819,7 @@
         <v>{ id: 183, name: 'Escuela de python 2021: Aprende python 3.9+ de cero a Master', category: 'Back-end', technology: 'python', url: 'https://www.udemy.com/course/curso-python-desde-cero', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 1260, culminado: null, certificado: '', url_certificado: '', instructor: 'Alex Roel Code', description: 'Curso de python 2021 : Aprende python con flask, django, Web Scraping, Data Science y mysql,HTML, css, bootstrap', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'python' ], mostrar: false, repositorio: '', nota: 'Este curso lo tiene María Valentina.' },</v>
       </c>
     </row>
-    <row r="185" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A185" s="6">
         <v>184</v>
       </c>
@@ -37972,7 +37984,7 @@
         <v>{ id: 184, name: 'Iniciación gerencial en el manejo de recursos en actividades socio – culturales', category: 'Otros', technology: 'Otros', url: '', platform: 'Centro de Orientación y Especialización Profesional', costo: 0, money: 'VEB', comprado: true, priority: 0, minutos: 480, culminado: '1994-02-19', certificado: '', url_certificado: '', instructor: 'María Mercedes Combes', description: 'Curso generencial. Centro de Orientación y Especialización Profesional. Mercedes Combes.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'generico', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="186" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A186" s="6">
         <v>185</v>
       </c>
@@ -38137,7 +38149,7 @@
         <v>{ id: 185, name: 'Introducción a la Programación en Fortran 95', category: 'Lenguajes de Programación', technology: 'Fortran', url: '', platform: 'Universidad Central de Venezuela', costo: 0, money: 'VEB', comprado: true, priority: 0, minutos: 128, culminado: '2002-02-01', certificado: '', url_certificado: '', instructor: 'Facultad de Ingeniería UCV', description: 'Curso de programación en Fortran 95. U.C.V., Facultad de Ingeniería. Instituto Tecnológico. Cursos de Extensión Profesional.', url_aux: '', calificacion: 'Muy bueno', actualizado: false, en_ruta: false, logo_platform: 'ucv', logo_technologies: [ 'fortran' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="187" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A187" s="6">
         <v>186</v>
       </c>
@@ -38302,7 +38314,7 @@
         <v>{ id: 186, name: 'Defensive Driving Certificate', category: 'Otros', technology: 'Otros', url: '', platform: 'ENI', costo: 0, money: 'VEB', comprado: true, priority: 0, minutos: 480, culminado: '2004-09-06', certificado: '', url_certificado: '', instructor: 'Luis Rosillo', description: 'ENI Dacion B.V. San Tomé. Estado Anzoátegui. Curso de manejo defensivo y comentado.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'eni', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="188" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A188" s="6">
         <v>187</v>
       </c>
@@ -38467,7 +38479,7 @@
         <v>{ id: 187, name: 'Deshidratación de Gas', category: 'Otros', technology: 'Otros', url: '', platform: 'Proynca', costo: 0, money: 'VEB', comprado: true, priority: 0, minutos: 1440, culminado: '2005-09-23', certificado: '', url_certificado: '', instructor: 'Rigoberto Brito', description: 'PROYNCA (Procesos y Negocios Integrales). San Tomé. Estado Anzoátegui. Dictado por el Ing. Rigoberto Brito.', url_aux: '', calificacion: 'Muy bueno', actualizado: false, en_ruta: false, logo_platform: 'proynca', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="189" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A189" s="6">
         <v>188</v>
       </c>
@@ -38632,7 +38644,7 @@
         <v>{ id: 188, name: 'Tratamiento de Aguas Efluentes', category: 'Otros', technology: 'Otros', url: '', platform: 'Proynca', costo: 0, money: 'VEB', comprado: true, priority: 0, minutos: 1440, culminado: '2005-10-14', certificado: '', url_certificado: '', instructor: 'Schacklanye Barradas', description: 'PROYNCA (Procesos y Negocios Integrales). San Tomé. Estado Anzoátegui. Dictado por la Ing. Schacklanye Barradas y la Ing. Emerita Machado.', url_aux: '', calificacion: 'Muy bueno', actualizado: false, en_ruta: false, logo_platform: 'proynca', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="190" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A190" s="6">
         <v>189</v>
       </c>
@@ -38797,7 +38809,7 @@
         <v>{ id: 189, name: 'Introducción a Medición de Variables de Proceso', category: 'Otros', technology: 'Otros', url: '', platform: 'ENI', costo: 0, money: 'VEB', comprado: true, priority: 0, minutos: 480, culminado: '2005-11-11', certificado: '', url_certificado: '', instructor: 'José David De Sousa', description: 'ENI Dacion B.V. San Tomé. Estado Anzoátegui. Curso de Medición de Variables, dictado por el Ing. José David De Sousa.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'eni', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="191" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A191" s="6">
         <v>190</v>
       </c>
@@ -38962,7 +38974,7 @@
         <v>{ id: 190, name: 'Deshidratación de Crudo', category: 'Otros', technology: 'Otros', url: '', platform: 'Proynca', costo: 0, money: 'VEB', comprado: true, priority: 0, minutos: 1440, culminado: '2005-11-25', certificado: '', url_certificado: '', instructor: 'Mercedes de Velázquez', description: 'PROYNCA (Procesos y Negocios Integrales). San Tomé. Estado Anzoátegui. Dictado por la Ing. Mercedes de Velázquez.', url_aux: '', calificacion: 'Muy bueno', actualizado: false, en_ruta: false, logo_platform: 'proynca', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="192" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A192" s="6">
         <v>191</v>
       </c>
@@ -39127,7 +39139,7 @@
         <v>{ id: 191, name: 'Seguridad en la Conducción de Vehículos', category: 'Otros', technology: 'Otros', url: '', platform: 'PDVSA', costo: 0, money: 'VEB', comprado: true, priority: 0, minutos: 960, culminado: '2006-08-16', certificado: '', url_certificado: '', instructor: 'Harold Pérez Fernández', description: 'PDVSA. San Tomé. Estado Anzoátegui. Curso de Manejo Defensivo (Flota Liviana), dictado por la Ing. Harold Pérez Fernández.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'pdvsa', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="193" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A193" s="6">
         <v>192</v>
       </c>
@@ -39292,7 +39304,7 @@
         <v>{ id: 192, name: 'Ortografía y Redacción de Informes', category: 'Otros', technology: 'Otros', url: '', platform: 'PDVSA', costo: 0, money: 'VEB', comprado: true, priority: 0, minutos: 960, culminado: '2007-02-16', certificado: '', url_certificado: '', instructor: 'PDVSA', description: 'Curso sobre ortografía y redacción de informes, orientado a profesionales de la industria petrolera. PDVSA. San Tomé. Estado Anzoátegui.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'pdvsa', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="194" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A194" s="6">
         <v>193</v>
       </c>
@@ -39457,7 +39469,7 @@
         <v>{ id: 193, name: 'Redacción de informes', category: 'Otros', technology: 'Otros', url: '', platform: 'PDVSA', costo: 0, money: 'VEB', comprado: true, priority: 0, minutos: 960, culminado: '2007-03-14', certificado: '', url_certificado: '', instructor: 'PDVSA', description: 'Curso sobre ortografía, orientado a profesionales de la industria petrolera. PDVSA. San Tomé. Estado Anzoátegui.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'pdvsa', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="195" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A195" s="6">
         <v>194</v>
       </c>
@@ -39622,7 +39634,7 @@
         <v>{ id: 194, name: 'La seguridad, la higiene y el ambiente en la industria (módulo C)', category: 'Otros', technology: 'Otros', url: '', platform: 'PDVSA', costo: 0, money: 'VEB', comprado: true, priority: 0, minutos: 2400, culminado: '2007-06-29', certificado: '', url_certificado: '', instructor: 'PDVSA', description: 'Curso sobre la seguridad, la higiene y el ambiente en la industria petrolera. PDVSA. San Tomé. Estado Anzoátegui.', url_aux: '', calificacion: 'Muy bueno', actualizado: false, en_ruta: false, logo_platform: 'pdvsa', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="196" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A196" s="6">
         <v>195</v>
       </c>
@@ -39787,7 +39799,7 @@
         <v>{ id: 195, name: 'Formulación de proyectos socio comunitarios', category: 'Otros', technology: 'Otros', url: '', platform: 'Mauritia, Consultores C.A.', costo: 0, money: 'VEB', comprado: true, priority: 0, minutos: 1200, culminado: '2007-09-20', certificado: '', url_certificado: '', instructor: 'Mauritia, Consultores C.A.', description: 'Mauritia, Consultores C.A. San Tomé. Estado Anzoátegui.', url_aux: '', calificacion: 'Bueno', actualizado: false, en_ruta: false, logo_platform: 'mauritia', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="197" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A197" s="6">
         <v>196</v>
       </c>
@@ -39952,7 +39964,7 @@
         <v>{ id: 196, name: 'Motivación para la calidad del trabajo', category: 'Otros', technology: 'Otros', url: '', platform: 'Gerencia Activa', costo: 0, money: 'VEB', comprado: true, priority: 0, minutos: 960, culminado: '2007-10-11', certificado: '', url_certificado: '', instructor: 'Gerencia Activa', description: 'Gerencia Activa. San Tomé. Estado Anzoátegui.', url_aux: '', calificacion: 'Bueno', actualizado: false, en_ruta: false, logo_platform: 'gerencia_activa', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="198" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A198" s="6">
         <v>197</v>
       </c>
@@ -40117,7 +40129,7 @@
         <v>{ id: 197, name: 'Corresponsabilidad en la toma de decisiones y solución de problemas', category: 'Otros', technology: 'Otros', url: '', platform: 'PDVSA', costo: 0, money: 'VEB', comprado: true, priority: 0, minutos: 960, culminado: '2007-12-12', certificado: '', url_certificado: '', instructor: 'PDVSA', description: 'PDVSA. San Tomé. Estado Anzoátegui.', url_aux: '', calificacion: 'Bueno', actualizado: false, en_ruta: false, logo_platform: 'pdvsa', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="199" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A199" s="6">
         <v>198</v>
       </c>
@@ -40282,7 +40294,7 @@
         <v>{ id: 198, name: 'Microsoft Project', category: 'Otros', technology: 'Otros', url: '', platform: 'PDVSA', costo: 0, money: 'VEF', comprado: true, priority: 0, minutos: 1440, culminado: '2009-09-10', certificado: '', url_certificado: '', instructor: 'Luis Carrion', description: 'Curso completo sobre Microsoft Proyect. PDVSA. San Tomé. Estado Anzoátegui.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'pdvsa', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="200" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A200" s="6">
         <v>199</v>
       </c>
@@ -40447,7 +40459,7 @@
         <v>{ id: 199, name: 'Potenciando mi rol de colaborador', category: 'Otros', technology: 'Otros', url: '', platform: 'Grupo Inested', costo: 0, money: 'VEF', comprado: true, priority: 0, minutos: 1440, culminado: '2016-10-05', certificado: '', url_certificado: '', instructor: 'Grupo Inested', description: 'Grupo Inested. PDVSA La Tahona.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'inested', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="201" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A201" s="6">
         <v>200</v>
       </c>
@@ -40612,7 +40624,7 @@
         <v>{ id: 200, name: 'Tecnología Petrolera', category: 'Otros', technology: 'Otros', url: '', platform: 'Seaport Agencies S.A.', costo: 0, money: 'VEF', comprado: true, priority: 0, minutos: 960, culminado: '2017-02-09', certificado: '', url_certificado: '', instructor: 'Seaport Agencies S.A.', description: 'Seaport Agencies S.A. Chacao. Torre La Primera.', url_aux: '', calificacion: 'Bueno', actualizado: false, en_ruta: false, logo_platform: 'seaport', logo_technologies: [ 'generico' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="202" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A202" s="5">
         <v>201</v>
       </c>
@@ -40776,7 +40788,7 @@
         <v>{ id: 201, name: 'Curso php 8 y mysql 8 desde cero', category: 'Back-end', technology: 'php', url: 'https://www.youtube.com/playlist?list=PLZ2ovOgdI-kUSqWuyoGJMZL6xldXw6hIg', platform: 'YouTube', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 705, culminado: null, certificado: '', url_certificado: '', instructor: 'Victor Arana Flores', description: 'Curso completo sobre php 8 y mysql 8 desde cero.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'youtube', logo_technologies: [ 'php','mysql' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="203" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A203" s="5">
         <v>202</v>
       </c>
@@ -40940,7 +40952,7 @@
         <v>{ id: 202, name: 'Universidad Visual Basic. net y sqlserver: De 0 a Experto', category: 'Frameworks de back-end', technology: '.NET', url: 'https://www.udemy.com/course/migrar-a-c-en-poco-tiempo', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 1733, culminado: null, certificado: '', url_certificado: '', instructor: 'Academia Apps', description: 'Curso Completo.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'vb','net','sqlserver' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="204" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A204" s="5">
         <v>203</v>
       </c>
@@ -41104,7 +41116,7 @@
         <v>{ id: 203, name: 'Curso de C# .NET desde cero hasta lo mas avanzado full stack', category: 'Frameworks de back-end', technology: '.NET', url: 'https://www.udemy.com/course/curso-de-c-sharp-net-core-desde-cero', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 1405, culminado: null, certificado: '', url_certificado: '', instructor: 'Alex Joel Pagoada Suazo', description: 'Curso de C# .NET desde cero para el desarrollo de diversas aplicaciones multiplataforma.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'csharp','net' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="205" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A205" s="5">
         <v>204</v>
       </c>
@@ -41268,7 +41280,7 @@
         <v>{ id: 204, name: 'Curso de C# y Net Core desde cero a nivel avanzado', category: 'Frameworks de back-end', technology: '.NET', url: 'https://www.udemy.com/course/curso-net', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 551, culminado: null, certificado: '', url_certificado: '', instructor: 'Vaxi Drez Arcila', description: 'Aprende C# | Programacion Orientada a Objetos| Net Core con Visual Studio 2022.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'csharp','net' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="206" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A206" s="5">
         <v>205</v>
       </c>
@@ -41432,7 +41444,7 @@
         <v>{ id: 205, name: 'CRUD con C# .NET 2021, 4 Capas, mysql, Win Form', category: 'Frameworks de back-end', technology: '.NET', url: 'https://www.udemy.com/course/crud-con-c-net-2021-4-capas-mysql-win-form', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 95, culminado: null, certificado: '', url_certificado: '', instructor: 'Joel Barrios (Bachi)', description: 'Aprende todo lo necesario para crear tus propios CRUD con C# .NET Gratis.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'csharp','net','mysql' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="207" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A207" s="5">
         <v>206</v>
       </c>
@@ -41596,7 +41608,7 @@
         <v>{ id: 206, name: 'CRUD con Visual Basic .NET 2021, 4 Capas, mysql, Win Form', category: 'Frameworks de back-end', technology: '.NET', url: 'https://www.udemy.com/course/crud-con-visual-basic-net-2021-4-capas', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 83, culminado: null, certificado: '', url_certificado: '', instructor: 'Joel Barrios (Bachi)', description: 'Aprende todo lo necesario para crear tus propios CRUD con Visual Basic .NET Gratis.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'vb','net','mysql' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="208" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A208" s="5">
         <v>207</v>
       </c>
@@ -41760,7 +41772,7 @@
         <v>{ id: 207, name: 'Desarrollo Web en ASP.NET CORE 5 (2021)', category: 'Frameworks de back-end', technology: '.NET', url: 'https://www.udemy.com/course/desarrollo-web-en-aspnet-core-5-2021', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 93, culminado: null, certificado: '', url_certificado: '', instructor: 'Carlos Piedra', description: 'Sistema de Control de Ingresos y Gastos - Full-Stack Web con .Net 5.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'net_core','sqlserver' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="209" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A209" s="10">
         <v>208</v>
       </c>
@@ -41924,7 +41936,7 @@
         <v>{ id: 208, name: 'Curso de Programación Orientada a Objetos con Ruby desde 0', category: 'Back-end', technology: 'Ruby', url: 'https://www.udemy.com/course/ruby-poo', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: false, priority: 0, minutos: 482, culminado: null, certificado: '', url_certificado: '', instructor: 'Pedro Vargas', description: 'Domina el Lenguaje de Programación Ruby! Curso Práctico de Ruby desde las bases de la programación hasta POO.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'ruby' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="210" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A210" s="10">
         <v>209</v>
       </c>
@@ -42088,7 +42100,7 @@
         <v>{ id: 209, name: 'Curso profesional de Ruby on Rails', category: 'Frameworks de back-end', technology: 'Rails', url: 'https://codigofacilito.com/cursos/rails-profesional', platform: 'Códigofacilito', costo: 20, money: 'EUR', comprado: true, priority: 0, minutos: 652, culminado: null, certificado: '', url_certificado: '', instructor: 'Uriel Hernández', description: 'Aprende a fondo y desde 0 Ruby on Rails. Es uno de los frameworks backend más importantes en la historia de la web, hoy Shopify, GitHub, Airbnb y otras empresas siguen usando Rails.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'codigofacilito', logo_technologies: [ 'ruby','rails' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="211" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A211" s="6">
         <v>210</v>
       </c>
@@ -42264,7 +42276,7 @@
         <v>{ id: 210, name: 'Nuxt.js - Framework de Vue.js con Strapi GraphQL', category: 'Frameworks de JavaScript', technology: 'Nuxt', url: 'https://www.udemy.com/course/nuxtjs-framework-de-vuejs-con-strapi-graphql/', platform: 'Udemy', costo: 12.99, money: 'EUR', comprado: true, priority: 0, minutos: 541, culminado: '2022-04-09', certificado: 'UC-b8541f71-23d7-4c12-9580-ff421f939bb7', url_certificado: 'https://www.udemy.com/certificate/UC-b8541f71-23d7-4c12-9580-ff421f939bb7', instructor: 'Santiago Catano Arango', description: '¡Aprende a crear aplicaciones Vue.js con Nuxt.js utilizando como base de datos Strapi GraphQL!', url_aux: '', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'nuxt','vuejs','graphql','strapi' ], mostrar: true, repositorio: 'https://github.com/petrix12/nuxt2022', nota: '' },</v>
       </c>
     </row>
-    <row r="212" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A212" s="7">
         <v>211</v>
       </c>
@@ -42428,7 +42440,7 @@
         <v>{ id: 211, name: 'Registro y Login con Redes Sociales PHP, MySQL y Firebase', category: 'Back-end', technology: 'Login', url: 'https://www.udemy.com/course/registro-y-login-con-redes-sociales-php-mysql-y-firebase', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 1, minutos: 156, culminado: null, certificado: '', url_certificado: '', instructor: 'Davis Anderson Bastidas Vicente', description: 'Registro y Login con Google, Facebook y Github.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'php','mysql','javascript','facebook','google','fireabase' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="213" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A213" s="6">
         <v>212</v>
       </c>
@@ -42604,7 +42616,7 @@
         <v>{ id: 212, name: 'Node: De cero a experto', category: 'Back-end', technology: 'Node.js', url: 'https://www.udemy.com/course/node-de-cero-a-experto', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 0, minutos: 1715, culminado: '2022-11-08', certificado: 'UC-b3413c5e-32df-47cf-b0e8-1d2824ce817a', url_certificado: 'https://udemy-certificate.s3.amazonaws.com/pdf/UC-b3413c5e-32df-47cf-b0e8-1d2824ce817a.pdf', instructor: 'Fernando Herrera', description: 'Rest, despliegues, Heroku, Mongo, Git, GitHub, Sockets, archivos, JWT y mucho más para ser un experto en Node.', url_aux: '', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'nodejs','mongo','javascript','git','github','heroku' ], mostrar: true, repositorio: 'https://github.com/petrix12/nodejs2022', nota: '' },</v>
       </c>
     </row>
-    <row r="214" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A214" s="6">
         <v>213</v>
       </c>
@@ -42780,7 +42792,7 @@
         <v>{ id: 213, name: 'Curso práctico de Docker y Microservicios (apto para todos)', category: 'Herramientas', technology: 'Docker', url: 'https://www.udemy.com/course/curso-practico-de-docker-y-microservicios-desde-cero', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: true, priority: 0, minutos: 535, culminado: '2022-12-27', certificado: 'UC-d479ccde-befd-4a7d-9632-5b1debb609e0', url_certificado: 'https://udemy-certificate.s3.amazonaws.com/pdf/UC-d479ccde-befd-4a7d-9632-5b1debb609e0.pdf', instructor: 'Juan Ramos', description: 'Aprende por qué es importante, cómo funciona, y cómo empezar usar Docker en tus proyectos!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'docker','laravel','mongo','python','mysql' ], mostrar: true, repositorio: 'https://github.com/petrix12/docker2022', nota: '' },</v>
       </c>
     </row>
-    <row r="215" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A215" s="5">
         <v>214</v>
       </c>
@@ -42944,7 +42956,7 @@
         <v>{ id: 214, name: 'Aprende lenguaje GO (GOLANG) desde 0', category: 'Back-end', technology: 'Golang', url: 'https://www.udemy.com/course/lenguaje-go', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 904, culminado: null, certificado: '', url_certificado: '', instructor: 'Pablo Tilotta', description: 'Toda la Sintaxis, estructuras y secretos del lenguaje GOLANG.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'golang' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="216" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A216" s="5">
         <v>215</v>
       </c>
@@ -43108,7 +43120,7 @@
         <v>{ id: 215, name: 'Aprende a programar con Go Golang', category: 'Back-end', technology: 'Golang', url: 'https://www.udemy.com/course/aprende-a-programar-con-go-golang', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 112, culminado: null, certificado: '', url_certificado: '', instructor: 'Proyecto Java', description: 'Aprende en 2 horas las bases de la programación informática y de la Programación Orientada a Objetos y la sintaxis de Go.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'golang' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="217" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A217" s="5">
         <v>216</v>
       </c>
@@ -43272,7 +43284,7 @@
         <v>{ id: 216, name: 'Universidad Java - De Cero a Experto - Más Completo +106 hrs', category: 'Back-end', technology: 'Java', url: 'https://www.udemy.com/course/universidad-java-especialista-en-java-desde-cero-a-master/learn/lecture/12885952?start=0#overview', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 6353, culminado: null, certificado: '', url_certificado: '', instructor: 'Ubaldo Acosta', description: 'El mejor curso de Java, POO, JDBC, Servlets, JavaEE, Web Services, JSF, EJB, JPA, PrimeFaces, Hibernate, Spring, Struts!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'java' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="218" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A218" s="5">
         <v>217</v>
       </c>
@@ -43436,7 +43448,7 @@
         <v>{ id: 217, name: 'PROBAR DJANGO | Crear una Aplicación Web', category: 'Back-end', technology: 'Django', url: 'https://www.udemy.com/course/probar-django-construir-una-aplicacion-web-en-python', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 266, culminado: null, certificado: '', url_certificado: '', instructor: 'Justin Mitchel', description: 'Curso de Django para principiantes: aprender lo básico para crear una página de aterrizaje dinámica en muy poco tiempo.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'django','phyton' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="219" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A219" s="5">
         <v>218</v>
       </c>
@@ -43600,7 +43612,7 @@
         <v>{ id: 218, name: 'Django 3- Python de cero (Ajax+Json+SQL Server+Bootstrap 5)', category: 'Back-end', technology: 'Django', url: 'https://www.udemy.com/course/django-3-python-de-cero-ajaxjsonsql-serverbootstrap-5', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 1519, culminado: null, certificado: '', url_certificado: '', instructor: 'Licito Hurol', description: 'Aprende a crear aplicaciones con Django y Sql Server usando Procedures , sin necesidad de tener conocimientos previos.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'django','phyton', 'sqlserver', 'bootstrap' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="220" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A220" s="5">
         <v>219</v>
       </c>
@@ -43764,7 +43776,7 @@
         <v>{ id: 219, name: 'Universidad Spring - Spring Framework y Spring Boot!', category: 'Frameworks de back-end', technology: 'Spring', url: 'https://www.udemy.com/course/universidad-spring-framework-springboot-java-security-rest-webservices', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 4455, culminado: null, certificado: '', url_certificado: '', instructor: 'Ubaldo Acosta', description: 'Aprende desde Cero hasta Experto el framework más popular de Java, Spring Framework con Spring Boot.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'spring' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="221" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A221" s="5">
         <v>220</v>
       </c>
@@ -43928,7 +43940,7 @@
         <v>{ id: 220, name: 'Bases de datos con MySQL y SQLite', category: 'Bases de datos', technology: 'MySQL', url: 'https://www.udemy.com/course/bases-de-datos-con-mysql-y-sqlite', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 950, culminado: null, certificado: '', url_certificado: '', instructor: 'Vladimir Rodríguez', description: 'Diseño y desarrollo de bases de datos relacionales en SQL de cero a PROFESIONAL.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'sql','mysql','sqlite' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="222" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A222" s="10">
         <v>221</v>
       </c>
@@ -44092,7 +44104,7 @@
         <v>{ id: 221, name: 'Aprende SQL usando PostgreSQL de cero', category: 'Bases de datos', technology: 'PostgreSQL', url: 'https://www.udemy.com/course/aprende-sql-usando-postgresql-de-cero-a-experto', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: false, priority: 0, minutos: 327, culminado: null, certificado: '', url_certificado: '', instructor: 'Andres Rojas', description: 'Aprende SQL desde cero para saber manejar cualquier base de datos usando PostgreSQL.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'postgresql' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="223" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A223" s="10">
         <v>222</v>
       </c>
@@ -44256,7 +44268,7 @@
         <v>{ id: 222, name: 'Base de datos con SQL Server administra y crea desde cero', category: 'Bases de datos', technology: 'SQL Server', url: 'https://www.udemy.com/course/database-sql-yoselerendon', platform: 'Udemy', costo: 9.99, money: 'EUR', comprado: false, priority: 0, minutos: 412, culminado: null, certificado: '', url_certificado: '', instructor: 'Yosele Rendon', description: 'Desarrolla, administra bases de datos, crea tablas, estructura tus columnas, programa con buenas practicas en campo real.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'sqlserver' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="224" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A224" s="5">
         <v>223</v>
       </c>
@@ -44420,7 +44432,7 @@
         <v>{ id: 223, name: 'MySQL para Principiantes , Introducción a las Bases de Datos', category: 'Bases de datos', technology: 'Maria DB', url: 'https://www.udemy.com/course/mysql-para-principiantes', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 114, culminado: null, certificado: '', url_certificado: '', instructor: 'Yury Zavaleta', description: 'MySQL desde cero , aprende los fundamentos de SQL y maneja de forma eficiente tu base de datos MySQL o Maria DB.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'mariadb','mysql' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="225" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A225" s="5">
         <v>224</v>
       </c>
@@ -44584,7 +44596,7 @@
         <v>{ id: 224, name: 'MongoDB: Aprende desde cero a experto', category: 'Bases de datos', technology: 'MongoDB', url: 'https://www.udemy.com/course/mongodb-aprende-desde-cero', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 443, culminado: null, certificado: '', url_certificado: '', instructor: 'Numpi Cursos', description: 'Vuelvete un experto en Bases de Datos no relacionales aprendiendo de una manera fácil y sencilla.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'mongodb' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="226" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A226" s="5">
         <v>225</v>
       </c>
@@ -44748,7 +44760,7 @@
         <v>{ id: 225, name: 'Procedimientos almacenados en PostgreSQL (PL/PgSQL)', category: 'Bases de datos', technology: 'PostgreSQL', url: 'https://www.udemy.com/course/procedimientos-almacenados-en-postgresql-plpgsql', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 163, culminado: null, certificado: '', url_certificado: '', instructor: 'Andres Rojas', description: 'Procedimientos almacenados.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'postgresql' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="227" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A227" s="5">
         <v>226</v>
       </c>
@@ -44912,7 +44924,7 @@
         <v>{ id: 226, name: 'GOLANG: Curso profesional de Go - De cero a Master 2022', category: 'Back-end', technology: 'Golang', url: 'https://www.udemy.com/course/curso-golang', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 877, culminado: null, certificado: '', url_certificado: '', instructor: 'Alex Roel Code', description: 'Aprende lenguaje de Go, Desarrollo Web con Go, Manejo de HTML, CSS, API RESTful com MySQL y ORM con Go', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'lgolang', 'mysql', 'html5', 'css' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="228" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A228" s="5">
         <v>227</v>
       </c>
@@ -45076,7 +45088,7 @@
         <v>{ id: 227, name: 'CodeIgniter 4 de cero a Experto. El mejor framework de PHP', category: 'Frameworks de back-end', technology: 'CodeIgniter', url: 'https://www.udemy.com/course/tutorial-codeigniter-4-de-cero-a-experto', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 264, culminado: null, certificado: '', url_certificado: '', instructor: 'David Navarro', description: 'CodeIgniter vuelve con una versión totalmente renovada. Aprende el mejor framework de PHP mientras programas un blog!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'codeIgniter' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="229" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A229" s="5">
         <v>228</v>
       </c>
@@ -45240,7 +45252,7 @@
         <v>{ id: 228, name: 'Guía definitiva para crear APIs con Symfony 5 y API Platform', category: 'Frameworks de back-end', technology: 'Symfony ', url: 'https://www.udemy.com/course/crear-api-con-symfony-y-api-platform', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 954, culminado: null, certificado: '', url_certificado: '', instructor: 'Juan González', description: 'Creación de una API con Symfony y API Platform. Estructura de servicios, RabbitMQ, Docker y mucho más!', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'apirestful','symfony' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="230" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A230" s="7">
         <v>229</v>
       </c>
@@ -45407,7 +45419,7 @@
         <v>{ id: 229, name: 'API REST Nodejs desde cero usando MongoDB o MySQL', category: 'Paradigmas', technology: 'API RESTful', url: 'https://www.udemy.com/course/api-rest-nodejs-desde-cero-usando-mongodb-o-mysql', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 1, minutos: 569, culminado: null, certificado: '', url_certificado: '', instructor: 'Leifer Mendez', description: '¿Cómo crear una API REST Nodejs usando MongoDB o MySQL? Incluye pruebas de integración (Testing)', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'udemy', logo_technologies: [ 'apirestful','nodejs','mongodb','mysql' ], mostrar: true, repositorio: 'https://github.com/petrix12/api_rest_nodejs_2022', nota: '' },</v>
       </c>
     </row>
-    <row r="231" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A231" s="6">
         <v>230</v>
       </c>
@@ -45583,7 +45595,7 @@
         <v>{ id: 230, name: 'Introducción a la programación', category: 'Paradigmas', technology: 'Lógica de programación', url: 'https://campus.open-bootcamp.com/cursos/3', platform: 'OpenBootcamp', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 573, culminado: '2022-05-31', certificado: '2F3051e4d4-08f0-494d-a8c7-4b6a7ad5fddf', url_certificado: 'https://storage.googleapis.com/openvitae-prod/diplomas%2F3051e4d4-08f0-494d-a8c7-4b6a7ad5fddf.pdf', instructor: 'Víctor Román Archidona', description: 'En este módulo aprenderéis las bases de la programación desde cero para que, sea cual sea el lenguaje que queráis abordar, tengáis claros los conceptos.', url_aux: '', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'openbootcamp', logo_technologies: [ 'java' ], mostrar: false, repositorio: 'https://github.com/petrix12/openbootcamp2022/blob/main/apuntes/001_introduccion_a_la_programacion.md', nota: '' },</v>
       </c>
     </row>
-    <row r="232" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A232" s="7">
         <v>231</v>
       </c>
@@ -45747,7 +45759,7 @@
         <v>{ id: 231, name: 'Angular para principiantes: Crea una aplicación real', category: 'Frameworks de JavaScript', technology: 'angular', url: 'https://www.udemy.com/course/angular-principiantes-leifer-mendez', platform: 'Udemy', costo: 0, money: 'EUR', comprado: true, priority: 1, minutos: 791, culminado: null, certificado: '', url_certificado: '', instructor: 'Leifer Mendez', description: 'Aprende a crear una aplicación increíble, la cual te servirá como portafolio y demostrar tus habilidades.', url_aux: '', calificacion: '*En evaluación*', actualizado: true, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'angular' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="233" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A233" s="6">
         <v>232</v>
       </c>
@@ -45923,7 +45935,7 @@
         <v>{ id: 232, name: 'Python Básico', category: 'Lenguajes de Programación', technology: 'Python', url: 'https://campus.open-bootcamp.com/cursos/6', platform: 'OpenBootcamp', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 835, culminado: '2022-05-31', certificado: '2F58f2a277-ffb5-4533-a9b9-c8d32c5c24d1', url_certificado: 'https://storage.googleapis.com/openvitae-prod/diplomas%2F58f2a277-ffb5-4533-a9b9-c8d32c5c24d1.pdf', instructor: 'Víctor Román Archidona', description: 'Lenguaje de programación interpretado que tiene como máxima destacar por una sintaxis que favorezca la legibilidad del código. Se trata de un lenguaje que soporta varios paradigmas tales como POO, programación imperativa y funcional.', url_aux: '', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'openbootcamp', logo_technologies: [ 'python' ], mostrar: false, repositorio: 'https://github.com/petrix12/openbootcamp2022/blob/main/apuntes/002_python.md', nota: '' },</v>
       </c>
     </row>
-    <row r="234" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A234" s="6">
         <v>233</v>
       </c>
@@ -46099,7 +46111,7 @@
         <v>{ id: 233, name: 'HTML y CSS Básico', category: 'Front-end', technology: 'General', url: 'https://campus.open-bootcamp.com/cursos/12', platform: 'OpenBootcamp', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 1063, culminado: '2022-06-21', certificado: '2F47303765-1db7-475e-b7f8-32f4a2d0f27d', url_certificado: 'https://storage.googleapis.com/openvitae-prod/diplomas%2F47303765-1db7-475e-b7f8-32f4a2d0f27d.pdf', instructor: 'Gorka Villar', description: 'Con este curso de HTML y CSS aprenderás las bases de todo desarrollo web, pues ambos son los lenguajes estándar para el desarrollo de páginas web en el mundo. Empieza a maquetar tus aplicaciones y páginas web de manera profesional desde 0.', url_aux: '', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'openbootcamp', logo_technologies: [ 'css','html5' ], mostrar: false, repositorio: 'https://github.com/petrix12/openbootcamp2022/blob/main/apuntes/003_html_y_css.md', nota: '' },</v>
       </c>
     </row>
-    <row r="235" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A235" s="6">
         <v>234</v>
       </c>
@@ -46275,7 +46287,7 @@
         <v>{ id: 234, name: 'JavaScript Básico', category: 'Front-end', technology: 'JavaScript', url: 'https://campus.open-bootcamp.com/cursos/15', platform: 'OpenBootcamp', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 924, culminado: '2022-07-04', certificado: '2F63bd7df1-d193-471c-b93c-87bcda39d678', url_certificado: 'https://storage.googleapis.com/openvitae-prod/diplomas%2F63bd7df1-d193-471c-b93c-87bcda39d678.pdf', instructor: 'Gorka Villar', description: 'Empieza tu formación en JavaScript, uno de los lenguajes más populares y utilizados en el desarrollo de aplicaciones web, multiplataforma, móvil y servicios, entre otros.', url_aux: '', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'openbootcamp', logo_technologies: [ 'javascript', 'nodejs' ], mostrar: false, repositorio: 'https://github.com/petrix12/openbootcamp2022/blob/main/apuntes/004_javascript_basico.md', nota: '' },</v>
       </c>
     </row>
-    <row r="236" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A236" s="6">
         <v>235</v>
       </c>
@@ -46451,7 +46463,7 @@
         <v>{ id: 235, name: 'Git', category: 'Herramientas', technology: 'Git', url: 'https://campus.open-bootcamp.com/cursos/10', platform: 'OpenBootcamp', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 976, culminado: '2022-07-14', certificado: '2F43f46455-8872-4e47-8fe1-8e18bf1f95b1', url_certificado: 'https://storage.googleapis.com/openvitae-prod/diplomas%2F43f46455-8872-4e47-8fe1-8e18bf1f95b1.pdf', instructor: 'Víctor Román Archidona', description: 'En este módulo aprenderás qué es un sistema de control de versiones y cómo gestionarlo de manera efectiva, junto a las herramientas más utilizada: Git, Gitlab, Github y Bitbucket. También aprenderás a automatizar procesos en pipelines de CI con tus repositorios remotos para empezar tu integración en el mundo de DevOps.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'openbootcamp', logo_technologies: [ 'git', 'github', 'gitlab', 'bitbucket' ], mostrar: false, repositorio: 'https://github.com/petrix12/openbootcamp2022/blob/main/apuntes/005_git.md', nota: '' },</v>
       </c>
     </row>
-    <row r="237" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A237" s="6">
         <v>236</v>
       </c>
@@ -46627,7 +46639,7 @@
         <v>{ id: 236, name: 'Java Básico', category: 'Lenguajes de Programación', technology: 'Java', url: 'https://campus.open-bootcamp.com/cursos/5', platform: 'OpenBootcamp', costo: 0, money: 'EUR', comprado: true, priority: 0, minutos: 893, culminado: '2022-09-08', certificado: '2Fb6e12ca9-6b3b-40bd-b690-b91d1c35f2a7', url_certificado: 'https://storage.googleapis.com/openvitae-prod/diplomas%2Fb6e12ca9-6b3b-40bd-b690-b91d1c35f2a7.pdf', instructor: 'Alan Sastre', description: 'Empieza tu formación desde 0 y domina tanto el lenguaje Java como las bases en la programación orientada a objetos.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: true, logo_platform: 'openbootcamp', logo_technologies: [ 'java' ], mostrar: false, repositorio: 'https://github.com/petrix12/openbootcamp2022/blob/main/apuntes/006_java_basico.md', nota: '' },</v>
       </c>
     </row>
-    <row r="238" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A238" s="6">
         <v>237</v>
       </c>
@@ -47315,7 +47327,7 @@
         <v>{ id: 240, name: 'Aprende a construir tu propio CMS con Laravel Voyager', category: 'Frameworks de back-end', technology: 'Laravel', url: 'https://codersfree.com/cursos/aprende-a-construir-tu-propio-cms-con-laravel-voyager', platform: 'Coders Free', costo: 14.99, money: 'USD', comprado: true, priority: 0, minutos: 234, culminado: '2022-10-16', certificado: 'S/C', url_certificado: '', instructor: 'Victor Arana Flores', description: 'En este curso aprenderás a construir tu propio CMS de una manera muy sencilla, gracias al paquete Laravel Voyager.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: false, logo_platform: 'coders_free', logo_technologies: [ 'laravel', 'voyager' ], mostrar: true, repositorio: 'https://github.com/petrix12/voyager2022', nota: '' },</v>
       </c>
     </row>
-    <row r="242" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A242" s="6">
         <v>241</v>
       </c>
@@ -47487,7 +47499,7 @@
         <v>{ id: 241, name: 'VuePress - Generador de Sitios Estáticos con Vue.js', category: 'Frameworks de JavaScript', technology: 'Vue JS', url: 'https://www.youtube.com/watch?v=o334x1W_RDY', platform: 'YouTube', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 25, culminado: '2022-11-07', certificado: 'S/C', url_certificado: '', instructor: 'Ignacio Gutiérrez ', description: 'Aprende a utilizar VuePress para tus próximos sitios web estáticos, este tutorial en español te mostrará los conceptos claves y fundamentos para montar tu sitio web a la velocidad de la luz.', url_aux: '', calificacion: 'Excelente', actualizado: false, en_ruta: false, logo_platform: 'youtube', logo_technologies: [ 'vuejs', 'vuepress' ], mostrar: false, repositorio: 'https://github.com/petrix12/vuepress2022', nota: '' },</v>
       </c>
     </row>
-    <row r="243" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A243" s="6">
         <v>242</v>
       </c>
@@ -47663,7 +47675,7 @@
         <v>{ id: 242, name: 'PWA - Aplicaciones Web Progresivas: De cero a experto', category: 'Herramientas', technology: 'PWA', url: 'https://www.udemy.com/course/aplicaciones-web-progresivas', platform: 'Udemy', costo: 12.99, money: 'EUR', comprado: true, priority: 0, minutos: 883, culminado: '2022-12-05', certificado: 'UC-08d71e30-3850-421f-92b6-690fcc31133b', url_certificado: 'https://udemy-certificate.s3.amazonaws.com/pdf/UC-08d71e30-3850-421f-92b6-690fcc31133b.pdf', instructor: 'Fernando Herrera', description: 'Notificaciones PUSH, sincronización sin conexión, modos offline, instalaciones, indexedDB, push server, share y más.', url_aux: '', calificacion: 'Muy bueno', actualizado: false, en_ruta: false, logo_platform: 'udemy', logo_technologies: [ 'pwa' ], mostrar: false, repositorio: 'https://github.com/petrix12/pwa2022', nota: '' },</v>
       </c>
     </row>
-    <row r="244" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A244" s="6">
         <v>243</v>
       </c>
@@ -48528,7 +48540,7 @@
         <v>{ id: 247, name: 'Aprende Laravel 10 desde cero', category: 'Frameworks de back-end', technology: 'Laravel', url: 'https://codersfree.com/cursos/aprende-laravel-desde-cero', platform: 'Coders Free', costo: 0, money: 'USD', comprado: false, priority: 0, minutos: 1332, culminado: '2023-07-24', certificado: 'S/C', url_certificado: '', instructor: 'Victor Arana Flores', description: 'Aprende Laravel 10 desde cero y conviértete en un experto en el framework PHP más popular. Construye aplicaciones web escalables y descubre las mejores prácticas y técnicas de Laravel. ¡Inscríbete ahora!', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: false, logo_platform: 'coders_free', logo_technologies: [ 'laravel' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
-    <row r="249" spans="1:52" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A249" s="6">
         <v>248</v>
       </c>
@@ -48906,10 +48918,10 @@
         <v>0</v>
       </c>
       <c r="K251">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="L251" s="9">
-        <v>45370</v>
+        <v>45377</v>
       </c>
       <c r="M251" t="s">
         <v>147</v>
@@ -48980,11 +48992,11 @@
       </c>
       <c r="AK251" t="str">
         <f>AK$1&amp;": "&amp;Tabla5[[#This Row],[minutos]]&amp;", "</f>
-        <v xml:space="preserve">minutos: 7, </v>
+        <v xml:space="preserve">minutos: 11, </v>
       </c>
       <c r="AL251" t="str">
         <f>AL$1&amp;": "&amp;IF(Tabla5[[#This Row],[culminado]]=0,"null","'"&amp;TEXT(Tabla5[[#This Row],[culminado]],"aaaa-mm-dd")&amp;"'")&amp;", "</f>
-        <v xml:space="preserve">culminado: '2024-03-19', </v>
+        <v xml:space="preserve">culminado: '2024-03-26', </v>
       </c>
       <c r="AM251" t="str">
         <f>AM$1&amp;": '"&amp;Tabla5[[#This Row],[certificado]]&amp;"', "</f>
@@ -49040,7 +49052,7 @@
       </c>
       <c r="AZ251" t="str">
         <f t="shared" si="33"/>
-        <v>{ id: 250, name: 'Novedades de Laravel 11', category: 'Frameworks de back-end', technology: 'Laravel', url: 'https://aprendible.com/series/novedades-de-laravel-11', platform: 'Aprendible', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 7, culminado: '2024-03-19', certificado: 'S/C', url_certificado: '', instructor: 'Jorge Luis García Coello', description: 'En esta serie de videos exploramos las últimas características de la versión 11 de Laravel y sus principales diferencias con la versión anterior.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'aprendible', logo_technologies: [ 'laravel' ], mostrar: false, repositorio: '', nota: '' },</v>
+        <v>{ id: 250, name: 'Novedades de Laravel 11', category: 'Frameworks de back-end', technology: 'Laravel', url: 'https://aprendible.com/series/novedades-de-laravel-11', platform: 'Aprendible', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 11, culminado: '2024-03-26', certificado: 'S/C', url_certificado: '', instructor: 'Jorge Luis García Coello', description: 'En esta serie de videos exploramos las últimas características de la versión 11 de Laravel y sus principales diferencias con la versión anterior.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'aprendible', logo_technologies: [ 'laravel' ], mostrar: false, repositorio: '', nota: '' },</v>
       </c>
     </row>
     <row r="252" spans="1:52" x14ac:dyDescent="0.3">
@@ -49099,7 +49111,7 @@
         <v>1364</v>
       </c>
       <c r="V252" s="19" t="s">
-        <v>1366</v>
+        <v>1372</v>
       </c>
       <c r="W252" s="19" t="s">
         <v>15</v>
@@ -49190,7 +49202,7 @@
       </c>
       <c r="AV252" t="str">
         <f>AV$1&amp;": [ "&amp;Tabla5[[#This Row],[logo_technologies]]&amp;" ], "</f>
-        <v xml:space="preserve">logo_technologies: [ arquitectura_hexagonal' ], </v>
+        <v xml:space="preserve">logo_technologies: [ 'arquitectura_hexagonal' ], </v>
       </c>
       <c r="AW252" t="str">
         <f>AW$1&amp;": "&amp;Tabla5[[#This Row],[mostrar]]&amp;", "</f>
@@ -49206,7 +49218,346 @@
       </c>
       <c r="AZ252" t="str">
         <f t="shared" si="33"/>
-        <v>{ id: 251, name: 'Arquitectura hexagonal', category: 'Paradigmas', technology: 'Programación', url: 'https://campus-ademass.com/curso/35', platform: 'Ademass', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 51, culminado: '2024-03-22', certificado: '', url_certificado: '', instructor: 'Juan José Ruíz Muñoz', description: 'Descubre cómo implementar la arquitectura hexagonal, también conocida como puertos y adaptadores, en tus proyectos de programación. Este video te proporcionará una sólida comprensión de los fundamentos teóricos detrás de esta arquitectura.', url_aux: '', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'ademass', logo_technologies: [ arquitectura_hexagonal' ], mostrar: false, repositorio: '', nota: '' },</v>
+        <v>{ id: 251, name: 'Arquitectura hexagonal', category: 'Paradigmas', technology: 'Programación', url: 'https://campus-ademass.com/curso/35', platform: 'Ademass', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 51, culminado: '2024-03-22', certificado: '', url_certificado: '', instructor: 'Juan José Ruíz Muñoz', description: 'Descubre cómo implementar la arquitectura hexagonal, también conocida como puertos y adaptadores, en tus proyectos de programación. Este video te proporcionará una sólida comprensión de los fundamentos teóricos detrás de esta arquitectura.', url_aux: '', calificacion: 'Muy bueno', actualizado: true, en_ruta: true, logo_platform: 'ademass', logo_technologies: [ 'arquitectura_hexagonal' ], mostrar: false, repositorio: '', nota: '' },</v>
+      </c>
+    </row>
+    <row r="253" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A253" s="6">
+        <v>252</v>
+      </c>
+      <c r="B253" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C253" t="s">
+        <v>333</v>
+      </c>
+      <c r="D253" t="s">
+        <v>332</v>
+      </c>
+      <c r="E253" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="F253" t="s">
+        <v>520</v>
+      </c>
+      <c r="G253" s="3">
+        <v>0</v>
+      </c>
+      <c r="H253" t="s">
+        <v>47</v>
+      </c>
+      <c r="I253" t="s">
+        <v>14</v>
+      </c>
+      <c r="J253" s="4">
+        <v>0</v>
+      </c>
+      <c r="K253">
+        <v>28</v>
+      </c>
+      <c r="L253" s="9">
+        <v>45377</v>
+      </c>
+      <c r="M253" t="s">
+        <v>147</v>
+      </c>
+      <c r="O253" t="s">
+        <v>1164</v>
+      </c>
+      <c r="P253" t="s">
+        <v>1368</v>
+      </c>
+      <c r="R253" t="s">
+        <v>458</v>
+      </c>
+      <c r="S253" t="s">
+        <v>14</v>
+      </c>
+      <c r="T253" t="s">
+        <v>14</v>
+      </c>
+      <c r="U253" t="s">
+        <v>764</v>
+      </c>
+      <c r="V253" s="19" t="s">
+        <v>839</v>
+      </c>
+      <c r="W253" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA253" t="str">
+        <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
+        <v xml:space="preserve">id: 252, </v>
+      </c>
+      <c r="AB253" t="str">
+        <f>AB$1&amp;": '"&amp;Tabla5[[#This Row],[name]]&amp;"', "</f>
+        <v xml:space="preserve">name: 'Novedades de Laravel 10', </v>
+      </c>
+      <c r="AC253" t="str">
+        <f>AC$1&amp;": '"&amp;Tabla5[[#This Row],[category]]&amp;"', "</f>
+        <v xml:space="preserve">category: 'Frameworks de back-end', </v>
+      </c>
+      <c r="AD253" t="str">
+        <f>AD$1&amp;": '"&amp;Tabla5[[#This Row],[technology]]&amp;"', "</f>
+        <v xml:space="preserve">technology: 'Laravel', </v>
+      </c>
+      <c r="AE253" t="str">
+        <f>AE$1&amp;": '"&amp;Tabla5[[#This Row],[url]]&amp;"', "</f>
+        <v xml:space="preserve">url: 'https://aprendible.com/series/novedades-de-laravel-10', </v>
+      </c>
+      <c r="AF253" t="str">
+        <f>AF$1&amp;": '"&amp;Tabla5[[#This Row],[platform]]&amp;"', "</f>
+        <v xml:space="preserve">platform: 'Aprendible', </v>
+      </c>
+      <c r="AG253" t="str">
+        <f>AG$1&amp;": "&amp;SUBSTITUTE(Tabla5[[#This Row],[costo]],",",".")&amp;", "</f>
+        <v xml:space="preserve">costo: 0, </v>
+      </c>
+      <c r="AH253" t="str">
+        <f>AH$1&amp;": '"&amp;Tabla5[[#This Row],[money]]&amp;"', "</f>
+        <v xml:space="preserve">money: 'USD', </v>
+      </c>
+      <c r="AI253" t="str">
+        <f>AI$1&amp;": "&amp;Tabla5[[#This Row],[comprado]]&amp;", "</f>
+        <v xml:space="preserve">comprado: true, </v>
+      </c>
+      <c r="AJ253" t="str">
+        <f>AJ$1&amp;": "&amp;Tabla5[[#This Row],[priority]]&amp;", "</f>
+        <v xml:space="preserve">priority: 0, </v>
+      </c>
+      <c r="AK253" t="str">
+        <f>AK$1&amp;": "&amp;Tabla5[[#This Row],[minutos]]&amp;", "</f>
+        <v xml:space="preserve">minutos: 28, </v>
+      </c>
+      <c r="AL253" t="str">
+        <f>AL$1&amp;": "&amp;IF(Tabla5[[#This Row],[culminado]]=0,"null","'"&amp;TEXT(Tabla5[[#This Row],[culminado]],"aaaa-mm-dd")&amp;"'")&amp;", "</f>
+        <v xml:space="preserve">culminado: '2024-03-26', </v>
+      </c>
+      <c r="AM253" t="str">
+        <f>AM$1&amp;": '"&amp;Tabla5[[#This Row],[certificado]]&amp;"', "</f>
+        <v xml:space="preserve">certificado: 'S/C', </v>
+      </c>
+      <c r="AN253" t="str">
+        <f>AN$1&amp;": '"&amp;Tabla5[[#This Row],[url_certificado]]&amp;"', "</f>
+        <v xml:space="preserve">url_certificado: '', </v>
+      </c>
+      <c r="AO253" t="str">
+        <f>AO$1&amp;": '"&amp;Tabla5[[#This Row],[instructor]]&amp;"', "</f>
+        <v xml:space="preserve">instructor: 'Jorge Luis García Coello', </v>
+      </c>
+      <c r="AP253" t="str">
+        <f>AP$1&amp;": '"&amp;Tabla5[[#This Row],[description]]&amp;"', "</f>
+        <v xml:space="preserve">description: 'En esta serie de videos exploramos las principales novedades de la versión 10 de Laravel liberada el 14 de febrero del 2023.', </v>
+      </c>
+      <c r="AQ253" t="str">
+        <f>AQ$1&amp;": '"&amp;Tabla5[[#This Row],[url_aux]]&amp;"', "</f>
+        <v xml:space="preserve">url_aux: '', </v>
+      </c>
+      <c r="AR253" t="str">
+        <f>AR$1&amp;": '"&amp;Tabla5[[#This Row],[calificacion]]&amp;"', "</f>
+        <v xml:space="preserve">calificacion: 'Excelente', </v>
+      </c>
+      <c r="AS253" t="str">
+        <f>AS$1&amp;": "&amp;Tabla5[[#This Row],[actualizado]]&amp;", "</f>
+        <v xml:space="preserve">actualizado: true, </v>
+      </c>
+      <c r="AT253" t="str">
+        <f>AT$1&amp;": "&amp;Tabla5[[#This Row],[en_ruta]]&amp;", "</f>
+        <v xml:space="preserve">en_ruta: true, </v>
+      </c>
+      <c r="AU253" t="str">
+        <f>AU$1&amp;": '"&amp;Tabla5[[#This Row],[logo_platform]]&amp;"', "</f>
+        <v xml:space="preserve">logo_platform: 'aprendible', </v>
+      </c>
+      <c r="AV253" t="str">
+        <f>AV$1&amp;": [ "&amp;Tabla5[[#This Row],[logo_technologies]]&amp;" ], "</f>
+        <v xml:space="preserve">logo_technologies: [ 'laravel' ], </v>
+      </c>
+      <c r="AW253" t="str">
+        <f>AW$1&amp;": "&amp;Tabla5[[#This Row],[mostrar]]&amp;", "</f>
+        <v xml:space="preserve">mostrar: false, </v>
+      </c>
+      <c r="AX253" t="str">
+        <f>AX$1&amp;": '"&amp;Tabla5[[#This Row],[repositorio]]&amp;"', "</f>
+        <v xml:space="preserve">repositorio: '', </v>
+      </c>
+      <c r="AY253" t="str">
+        <f>AY$1&amp;": '"&amp;Tabla5[[#This Row],[nota]]&amp;"'"</f>
+        <v>nota: ''</v>
+      </c>
+      <c r="AZ253" t="str">
+        <f t="shared" ref="AZ253" si="34">"{ "&amp;AA253&amp;AB253&amp;AC253&amp;AD253&amp;AE253&amp;AF253&amp;AG253&amp;AH253&amp;AI253&amp;AJ253&amp;AK253&amp;AL253&amp;AM253&amp;AN253&amp;AO253&amp;AP253&amp;AQ253&amp;AR253&amp;AS253&amp;AT253&amp;AU253&amp;AV253&amp;AW253&amp;AX253&amp;AY253&amp;" },"</f>
+        <v>{ id: 252, name: 'Novedades de Laravel 10', category: 'Frameworks de back-end', technology: 'Laravel', url: 'https://aprendible.com/series/novedades-de-laravel-10', platform: 'Aprendible', costo: 0, money: 'USD', comprado: true, priority: 0, minutos: 28, culminado: '2024-03-26', certificado: 'S/C', url_certificado: '', instructor: 'Jorge Luis García Coello', description: 'En esta serie de videos exploramos las principales novedades de la versión 10 de Laravel liberada el 14 de febrero del 2023.', url_aux: '', calificacion: 'Excelente', actualizado: true, en_ruta: true, logo_platform: 'aprendible', logo_technologies: [ 'laravel' ], mostrar: false, repositorio: '', nota: '' },</v>
+      </c>
+    </row>
+    <row r="254" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A254" s="6">
+        <v>253</v>
+      </c>
+      <c r="B254" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C254" t="s">
+        <v>333</v>
+      </c>
+      <c r="D254" t="s">
+        <v>332</v>
+      </c>
+      <c r="E254" s="2" t="s">
+        <v>1370</v>
+      </c>
+      <c r="F254" t="s">
+        <v>149</v>
+      </c>
+      <c r="G254" s="3">
+        <v>10</v>
+      </c>
+      <c r="H254" t="s">
+        <v>47</v>
+      </c>
+      <c r="I254" t="s">
+        <v>14</v>
+      </c>
+      <c r="J254" s="4">
+        <v>0</v>
+      </c>
+      <c r="K254">
+        <f>34.9*60</f>
+        <v>2094</v>
+      </c>
+      <c r="L254" s="9">
+        <v>45457</v>
+      </c>
+      <c r="M254" t="s">
+        <v>147</v>
+      </c>
+      <c r="O254" t="s">
+        <v>150</v>
+      </c>
+      <c r="P254" t="s">
+        <v>1371</v>
+      </c>
+      <c r="R254" t="s">
+        <v>446</v>
+      </c>
+      <c r="S254" t="s">
+        <v>14</v>
+      </c>
+      <c r="T254" t="s">
+        <v>15</v>
+      </c>
+      <c r="U254" t="s">
+        <v>767</v>
+      </c>
+      <c r="V254" s="19" t="s">
+        <v>839</v>
+      </c>
+      <c r="W254" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA254" t="str">
+        <f>AA$1&amp;": "&amp;Tabla5[[#This Row],[id]]&amp;", "</f>
+        <v xml:space="preserve">id: 253, </v>
+      </c>
+      <c r="AB254" t="str">
+        <f>AB$1&amp;": '"&amp;Tabla5[[#This Row],[name]]&amp;"', "</f>
+        <v xml:space="preserve">name: 'Curso avanzado de Laravel 11', </v>
+      </c>
+      <c r="AC254" t="str">
+        <f>AC$1&amp;": '"&amp;Tabla5[[#This Row],[category]]&amp;"', "</f>
+        <v xml:space="preserve">category: 'Frameworks de back-end', </v>
+      </c>
+      <c r="AD254" t="str">
+        <f>AD$1&amp;": '"&amp;Tabla5[[#This Row],[technology]]&amp;"', "</f>
+        <v xml:space="preserve">technology: 'Laravel', </v>
+      </c>
+      <c r="AE254" t="str">
+        <f>AE$1&amp;": '"&amp;Tabla5[[#This Row],[url]]&amp;"', "</f>
+        <v xml:space="preserve">url: 'https://codersfree.com/cursos/aprende-laravel-avanzado', </v>
+      </c>
+      <c r="AF254" t="str">
+        <f>AF$1&amp;": '"&amp;Tabla5[[#This Row],[platform]]&amp;"', "</f>
+        <v xml:space="preserve">platform: 'Coders Free', </v>
+      </c>
+      <c r="AG254" t="str">
+        <f>AG$1&amp;": "&amp;SUBSTITUTE(Tabla5[[#This Row],[costo]],",",".")&amp;", "</f>
+        <v xml:space="preserve">costo: 10, </v>
+      </c>
+      <c r="AH254" t="str">
+        <f>AH$1&amp;": '"&amp;Tabla5[[#This Row],[money]]&amp;"', "</f>
+        <v xml:space="preserve">money: 'USD', </v>
+      </c>
+      <c r="AI254" t="str">
+        <f>AI$1&amp;": "&amp;Tabla5[[#This Row],[comprado]]&amp;", "</f>
+        <v xml:space="preserve">comprado: true, </v>
+      </c>
+      <c r="AJ254" t="str">
+        <f>AJ$1&amp;": "&amp;Tabla5[[#This Row],[priority]]&amp;", "</f>
+        <v xml:space="preserve">priority: 0, </v>
+      </c>
+      <c r="AK254" t="str">
+        <f>AK$1&amp;": "&amp;Tabla5[[#This Row],[minutos]]&amp;", "</f>
+        <v xml:space="preserve">minutos: 2094, </v>
+      </c>
+      <c r="AL254" t="str">
+        <f>AL$1&amp;": "&amp;IF(Tabla5[[#This Row],[culminado]]=0,"null","'"&amp;TEXT(Tabla5[[#This Row],[culminado]],"aaaa-mm-dd")&amp;"'")&amp;", "</f>
+        <v xml:space="preserve">culminado: '2024-06-14', </v>
+      </c>
+      <c r="AM254" t="str">
+        <f>AM$1&amp;": '"&amp;Tabla5[[#This Row],[certificado]]&amp;"', "</f>
+        <v xml:space="preserve">certificado: 'S/C', </v>
+      </c>
+      <c r="AN254" t="str">
+        <f>AN$1&amp;": '"&amp;Tabla5[[#This Row],[url_certificado]]&amp;"', "</f>
+        <v xml:space="preserve">url_certificado: '', </v>
+      </c>
+      <c r="AO254" t="str">
+        <f>AO$1&amp;": '"&amp;Tabla5[[#This Row],[instructor]]&amp;"', "</f>
+        <v xml:space="preserve">instructor: 'Victor Arana Flores', </v>
+      </c>
+      <c r="AP254" t="str">
+        <f>AP$1&amp;": '"&amp;Tabla5[[#This Row],[description]]&amp;"', "</f>
+        <v xml:space="preserve">description: 'En este curso avanzado de Laravel 11, aprenderás técnicas y herramientas avanzadas para mejorar tus habilidades en Laravel. Domina Laravel y crea aplicaciones web de alta calidad.', </v>
+      </c>
+      <c r="AQ254" t="str">
+        <f>AQ$1&amp;": '"&amp;Tabla5[[#This Row],[url_aux]]&amp;"', "</f>
+        <v xml:space="preserve">url_aux: '', </v>
+      </c>
+      <c r="AR254" t="str">
+        <f>AR$1&amp;": '"&amp;Tabla5[[#This Row],[calificacion]]&amp;"', "</f>
+        <v xml:space="preserve">calificacion: 'Bueno', </v>
+      </c>
+      <c r="AS254" t="str">
+        <f>AS$1&amp;": "&amp;Tabla5[[#This Row],[actualizado]]&amp;", "</f>
+        <v xml:space="preserve">actualizado: true, </v>
+      </c>
+      <c r="AT254" t="str">
+        <f>AT$1&amp;": "&amp;Tabla5[[#This Row],[en_ruta]]&amp;", "</f>
+        <v xml:space="preserve">en_ruta: false, </v>
+      </c>
+      <c r="AU254" t="str">
+        <f>AU$1&amp;": '"&amp;Tabla5[[#This Row],[logo_platform]]&amp;"', "</f>
+        <v xml:space="preserve">logo_platform: 'coders_free', </v>
+      </c>
+      <c r="AV254" t="str">
+        <f>AV$1&amp;": [ "&amp;Tabla5[[#This Row],[logo_technologies]]&amp;" ], "</f>
+        <v xml:space="preserve">logo_technologies: [ 'laravel' ], </v>
+      </c>
+      <c r="AW254" t="str">
+        <f>AW$1&amp;": "&amp;Tabla5[[#This Row],[mostrar]]&amp;", "</f>
+        <v xml:space="preserve">mostrar: true, </v>
+      </c>
+      <c r="AX254" t="str">
+        <f>AX$1&amp;": '"&amp;Tabla5[[#This Row],[repositorio]]&amp;"', "</f>
+        <v xml:space="preserve">repositorio: '', </v>
+      </c>
+      <c r="AY254" t="str">
+        <f>AY$1&amp;": '"&amp;Tabla5[[#This Row],[nota]]&amp;"'"</f>
+        <v>nota: ''</v>
+      </c>
+      <c r="AZ254" t="str">
+        <f t="shared" ref="AZ254" si="35">"{ "&amp;AA254&amp;AB254&amp;AC254&amp;AD254&amp;AE254&amp;AF254&amp;AG254&amp;AH254&amp;AI254&amp;AJ254&amp;AK254&amp;AL254&amp;AM254&amp;AN254&amp;AO254&amp;AP254&amp;AQ254&amp;AR254&amp;AS254&amp;AT254&amp;AU254&amp;AV254&amp;AW254&amp;AX254&amp;AY254&amp;" },"</f>
+        <v>{ id: 253, name: 'Curso avanzado de Laravel 11', category: 'Frameworks de back-end', technology: 'Laravel', url: 'https://codersfree.com/cursos/aprende-laravel-avanzado', platform: 'Coders Free', costo: 10, money: 'USD', comprado: true, priority: 0, minutos: 2094, culminado: '2024-06-14', certificado: 'S/C', url_certificado: '', instructor: 'Victor Arana Flores', description: 'En este curso avanzado de Laravel 11, aprenderás técnicas y herramientas avanzadas para mejorar tus habilidades en Laravel. Domina Laravel y crea aplicaciones web de alta calidad.', url_aux: '', calificacion: 'Bueno', actualizado: true, en_ruta: false, logo_platform: 'coders_free', logo_technologies: [ 'laravel' ], mostrar: true, repositorio: '', nota: '' },</v>
       </c>
     </row>
   </sheetData>
@@ -49223,7 +49574,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{080BBF38-91CF-44A2-8034-B83AEB3677D2}">
       <formula1>platform</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:T1048576 I2:I1048576 W2:W1048576" xr:uid="{678243B2-4193-4FA8-A190-37A986A340CF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576 S2:T1048576 W2:W1048576" xr:uid="{678243B2-4193-4FA8-A190-37A986A340CF}">
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{FA3C4A9B-80C8-4335-B4E6-A3C8412DC1E8}">
@@ -49571,11 +49922,13 @@
     <hyperlink ref="E250" r:id="rId329" xr:uid="{4FD6D661-67A9-4D8C-B627-0ACC80A7F748}"/>
     <hyperlink ref="E251" r:id="rId330" xr:uid="{7A73DA1F-4125-4793-8DDA-DCE8B97B3494}"/>
     <hyperlink ref="E252" r:id="rId331" xr:uid="{702A05C3-C88F-43E5-827D-546D9E55EC24}"/>
+    <hyperlink ref="E253" r:id="rId332" xr:uid="{A960D24E-B223-4353-9235-6FC29EE7C375}"/>
+    <hyperlink ref="E254" r:id="rId333" xr:uid="{248FC9F0-067D-4CDA-AD75-BECE2BEBA591}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId332"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId334"/>
   <tableParts count="1">
-    <tablePart r:id="rId333"/>
+    <tablePart r:id="rId335"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>